<commit_message>
added in content ids
</commit_message>
<xml_diff>
--- a/Daisy-xls/IA/CTHP-Cards.xlsx
+++ b/Daisy-xls/IA/CTHP-Cards.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-500" windowWidth="28860" windowHeight="16540" tabRatio="655" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="-495" windowWidth="28860" windowHeight="16545" tabRatio="655" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="BRAIN" sheetId="6" r:id="rId1"/>
@@ -909,7 +909,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -928,6 +928,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1020,7 +1026,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1042,6 +1048,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1461,22 +1471,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection sqref="A1:XFD1"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="56.1640625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="56.125" style="2" customWidth="1"/>
     <col min="2" max="2" width="47.5" style="2" customWidth="1"/>
-    <col min="4" max="4" width="26.1640625" customWidth="1"/>
-    <col min="5" max="5" width="22.33203125" customWidth="1"/>
-    <col min="6" max="6" width="19.33203125" customWidth="1"/>
+    <col min="4" max="4" width="26.125" customWidth="1"/>
+    <col min="5" max="5" width="22.375" customWidth="1"/>
+    <col min="6" max="6" width="19.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="17.25">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1496,13 +1506,16 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="31.5">
+    <row r="2" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>139</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>140</v>
       </c>
+      <c r="C2">
+        <v>1040</v>
+      </c>
       <c r="D2" t="s">
         <v>33</v>
       </c>
@@ -1513,13 +1526,16 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="31.5">
+    <row r="3" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>141</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>142</v>
       </c>
+      <c r="C3">
+        <v>5102</v>
+      </c>
       <c r="D3" t="s">
         <v>33</v>
       </c>
@@ -1530,13 +1546,16 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="31.5">
+    <row r="4" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>143</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>144</v>
       </c>
+      <c r="C4">
+        <v>4722</v>
+      </c>
       <c r="D4" t="s">
         <v>33</v>
       </c>
@@ -1547,13 +1566,16 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="31.5">
+    <row r="5" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>145</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>146</v>
       </c>
+      <c r="C5">
+        <v>6395</v>
+      </c>
       <c r="D5" t="s">
         <v>33</v>
       </c>
@@ -1564,13 +1586,16 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="31.5">
+    <row r="6" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>147</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>148</v>
       </c>
+      <c r="C6">
+        <v>4266</v>
+      </c>
       <c r="D6" t="s">
         <v>33</v>
       </c>
@@ -1581,13 +1606,16 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="31.5">
+    <row r="7" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>149</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>150</v>
       </c>
+      <c r="C7">
+        <v>6413</v>
+      </c>
       <c r="D7" t="s">
         <v>33</v>
       </c>
@@ -1598,13 +1626,16 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="31.5">
+    <row r="8" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>151</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>152</v>
       </c>
+      <c r="C8">
+        <v>6311</v>
+      </c>
       <c r="D8" t="s">
         <v>33</v>
       </c>
@@ -1615,13 +1646,16 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="31.5">
+    <row r="9" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>153</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>154</v>
       </c>
+      <c r="C9">
+        <v>212044</v>
+      </c>
       <c r="D9" t="s">
         <v>33</v>
       </c>
@@ -1632,13 +1666,16 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="31.5">
+    <row r="10" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>155</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>156</v>
       </c>
+      <c r="C10">
+        <v>4426</v>
+      </c>
       <c r="D10" t="s">
         <v>33</v>
       </c>
@@ -1649,13 +1686,16 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="31.5">
+    <row r="11" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>157</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>158</v>
       </c>
+      <c r="C11">
+        <v>4426</v>
+      </c>
       <c r="D11" t="s">
         <v>33</v>
       </c>
@@ -1666,13 +1706,16 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="31.5">
+    <row r="12" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>159</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>160</v>
       </c>
+      <c r="C12">
+        <v>65187</v>
+      </c>
       <c r="D12" t="s">
         <v>161</v>
       </c>
@@ -1683,7 +1726,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>162</v>
       </c>
@@ -1701,7 +1744,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="31.5">
+    <row r="14" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>164</v>
       </c>
@@ -1719,7 +1762,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="31.5">
+    <row r="15" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>166</v>
       </c>
@@ -1737,7 +1780,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="31.5">
+    <row r="16" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>168</v>
       </c>
@@ -1755,7 +1798,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="31.5">
+    <row r="17" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>170</v>
       </c>
@@ -1773,7 +1816,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="31.5">
+    <row r="18" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>172</v>
       </c>
@@ -1791,7 +1834,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="31.5">
+    <row r="19" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>174</v>
       </c>
@@ -1809,7 +1852,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="31.5">
+    <row r="20" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>176</v>
       </c>
@@ -1827,7 +1870,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="31.5">
+    <row r="21" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>178</v>
       </c>
@@ -1845,7 +1888,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="31.5">
+    <row r="22" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>180</v>
       </c>
@@ -1863,7 +1906,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="31.5">
+    <row r="23" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>182</v>
       </c>
@@ -1881,7 +1924,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="31.5">
+    <row r="24" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>184</v>
       </c>
@@ -1899,7 +1942,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="31.5">
+    <row r="25" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>63</v>
       </c>
@@ -1919,7 +1962,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="31.5">
+    <row r="26" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>64</v>
       </c>
@@ -1939,7 +1982,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="31.5">
+    <row r="27" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>85</v>
       </c>
@@ -1959,7 +2002,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
         <v>186</v>
       </c>
@@ -1971,13 +2014,16 @@
         <v>41</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="31.5">
+    <row r="29" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>139</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>187</v>
       </c>
+      <c r="C29">
+        <v>3240</v>
+      </c>
       <c r="D29" t="s">
         <v>33</v>
       </c>
@@ -1988,13 +2034,16 @@
         <v>40</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="31.5">
+    <row r="30" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>141</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>188</v>
       </c>
+      <c r="C30">
+        <v>1666</v>
+      </c>
       <c r="D30" t="s">
         <v>33</v>
       </c>
@@ -2005,13 +2054,16 @@
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="31.5">
+    <row r="31" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>143</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>189</v>
       </c>
+      <c r="C31">
+        <v>997</v>
+      </c>
       <c r="D31" t="s">
         <v>33</v>
       </c>
@@ -2022,13 +2074,16 @@
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="31.5">
+    <row r="32" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>145</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>190</v>
       </c>
+      <c r="C32">
+        <v>6590</v>
+      </c>
       <c r="D32" t="s">
         <v>33</v>
       </c>
@@ -2039,13 +2094,16 @@
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="31.5">
+    <row r="33" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>147</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>191</v>
       </c>
+      <c r="C33">
+        <v>1601</v>
+      </c>
       <c r="D33" t="s">
         <v>33</v>
       </c>
@@ -2056,13 +2114,16 @@
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="31.5">
+    <row r="34" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>149</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>192</v>
       </c>
+      <c r="C34">
+        <v>6463</v>
+      </c>
       <c r="D34" t="s">
         <v>33</v>
       </c>
@@ -2073,13 +2134,16 @@
         <v>40</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="31.5">
+    <row r="35" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>151</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>193</v>
       </c>
+      <c r="C35">
+        <v>6293</v>
+      </c>
       <c r="D35" t="s">
         <v>33</v>
       </c>
@@ -2090,13 +2154,16 @@
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="31.5">
+    <row r="36" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>153</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>194</v>
       </c>
+      <c r="C36">
+        <v>145267</v>
+      </c>
       <c r="D36" t="s">
         <v>33</v>
       </c>
@@ -2107,13 +2174,16 @@
         <v>40</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="31.5">
+    <row r="37" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>155</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>195</v>
       </c>
+      <c r="C37">
+        <v>6476</v>
+      </c>
       <c r="D37" t="s">
         <v>33</v>
       </c>
@@ -2124,13 +2194,16 @@
         <v>40</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="31.5">
+    <row r="38" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>157</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>196</v>
       </c>
+      <c r="C38">
+        <v>2451</v>
+      </c>
       <c r="D38" t="s">
         <v>33</v>
       </c>
@@ -2141,7 +2214,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="31.5">
+    <row r="39" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>63</v>
       </c>
@@ -2161,7 +2234,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="31.5">
+    <row r="40" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>85</v>
       </c>
@@ -2196,20 +2269,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C2" sqref="C2:C31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="46" style="2" customWidth="1"/>
-    <col min="2" max="2" width="69.33203125" style="2" customWidth="1"/>
-    <col min="4" max="5" width="24.6640625" customWidth="1"/>
-    <col min="6" max="6" width="18.33203125" customWidth="1"/>
+    <col min="2" max="2" width="69.375" style="2" customWidth="1"/>
+    <col min="4" max="5" width="24.625" customWidth="1"/>
+    <col min="6" max="6" width="18.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="17.25">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2229,7 +2302,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>94</v>
       </c>
@@ -2249,7 +2322,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>96</v>
       </c>
@@ -2269,7 +2342,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>99</v>
       </c>
@@ -2289,7 +2362,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="31.5">
+    <row r="5" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>102</v>
       </c>
@@ -2309,7 +2382,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>105</v>
       </c>
@@ -2329,7 +2402,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>108</v>
       </c>
@@ -2349,7 +2422,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>111</v>
       </c>
@@ -2369,7 +2442,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>116</v>
       </c>
@@ -2389,7 +2462,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="31.5">
+    <row r="10" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>119</v>
       </c>
@@ -2407,7 +2480,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="31.5">
+    <row r="11" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>120</v>
       </c>
@@ -2425,7 +2498,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="31.5">
+    <row r="12" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>122</v>
       </c>
@@ -2443,7 +2516,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="31.5">
+    <row r="13" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>124</v>
       </c>
@@ -2461,7 +2534,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="31.5">
+    <row r="14" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>130</v>
       </c>
@@ -2479,7 +2552,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="31.5">
+    <row r="15" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>128</v>
       </c>
@@ -2497,7 +2570,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="31.5">
+    <row r="16" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>126</v>
       </c>
@@ -2515,7 +2588,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="31.5">
+    <row r="17" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>132</v>
       </c>
@@ -2533,7 +2606,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="31.5">
+    <row r="18" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>134</v>
       </c>
@@ -2551,7 +2624,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="31.5">
+    <row r="19" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>135</v>
       </c>
@@ -2569,7 +2642,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>63</v>
       </c>
@@ -2589,7 +2662,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>64</v>
       </c>
@@ -2609,7 +2682,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>85</v>
       </c>
@@ -2629,7 +2702,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
       <c r="B23" s="2" t="s">
         <v>138</v>
@@ -2642,7 +2715,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>94</v>
       </c>
@@ -2662,7 +2735,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>96</v>
       </c>
@@ -2682,7 +2755,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>99</v>
       </c>
@@ -2702,7 +2775,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="31.5">
+    <row r="27" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>102</v>
       </c>
@@ -2722,7 +2795,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>105</v>
       </c>
@@ -2742,7 +2815,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>108</v>
       </c>
@@ -2762,7 +2835,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="31.5">
+    <row r="30" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>111</v>
       </c>
@@ -2782,7 +2855,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>115</v>
       </c>
@@ -2802,7 +2875,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="31.5">
+    <row r="32" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>63</v>
       </c>
@@ -2822,7 +2895,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>85</v>
       </c>
@@ -2860,19 +2933,19 @@
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection sqref="A1:XFD1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.33203125" customWidth="1"/>
-    <col min="2" max="2" width="59.83203125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="40.375" customWidth="1"/>
+    <col min="2" max="2" width="59.875" style="2" customWidth="1"/>
     <col min="4" max="4" width="24" customWidth="1"/>
-    <col min="5" max="5" width="23.33203125" customWidth="1"/>
-    <col min="6" max="6" width="19.33203125" customWidth="1"/>
+    <col min="5" max="5" width="23.375" customWidth="1"/>
+    <col min="6" max="6" width="19.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="17.25">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2892,13 +2965,16 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>197</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>198</v>
       </c>
+      <c r="C2" s="2">
+        <v>4897</v>
+      </c>
       <c r="D2" t="s">
         <v>33</v>
       </c>
@@ -2909,13 +2985,16 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="31.5">
+    <row r="3" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>199</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>200</v>
       </c>
+      <c r="C3" s="2">
+        <v>4564</v>
+      </c>
       <c r="D3" t="s">
         <v>33</v>
       </c>
@@ -2926,13 +3005,16 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>201</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>202</v>
       </c>
+      <c r="C4" s="2">
+        <v>5220</v>
+      </c>
       <c r="D4" t="s">
         <v>33</v>
       </c>
@@ -2943,7 +3025,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="31.5">
+    <row r="5" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>203</v>
       </c>
@@ -2961,14 +3043,16 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>205</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="C6" s="9"/>
+      <c r="C6" s="2">
+        <v>102660</v>
+      </c>
       <c r="D6" t="s">
         <v>29</v>
       </c>
@@ -2979,14 +3063,16 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>207</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="C7" s="9"/>
+      <c r="C7" s="2">
+        <v>15469</v>
+      </c>
       <c r="D7" t="s">
         <v>29</v>
       </c>
@@ -2997,7 +3083,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
@@ -3017,14 +3103,16 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="31.5">
+    <row r="9" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>209</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="C9" s="2"/>
+      <c r="C9" s="2">
+        <v>5913</v>
+      </c>
       <c r="D9" s="2" t="s">
         <v>50</v>
       </c>
@@ -3035,7 +3123,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>63</v>
       </c>
@@ -3055,7 +3143,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="31.5">
+    <row r="11" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>64</v>
       </c>
@@ -3075,13 +3163,16 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="31.5">
+    <row r="12" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>211</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>212</v>
       </c>
+      <c r="C12" s="2">
+        <v>5913</v>
+      </c>
       <c r="D12" t="s">
         <v>51</v>
       </c>
@@ -3092,14 +3183,14 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>85</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="2">
         <v>6145</v>
       </c>
       <c r="D13" t="s">
@@ -3112,13 +3203,16 @@
         <v>84</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="31.5">
+    <row r="14" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>213</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>214</v>
       </c>
+      <c r="C14" s="2">
+        <v>13674</v>
+      </c>
       <c r="D14" t="s">
         <v>29</v>
       </c>
@@ -3129,7 +3223,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
       <c r="B15" s="2" t="s">
         <v>215</v>
@@ -3142,13 +3236,16 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="31.5">
+    <row r="16" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>197</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>216</v>
       </c>
+      <c r="C16" s="2">
+        <v>3341</v>
+      </c>
       <c r="D16" t="s">
         <v>33</v>
       </c>
@@ -3159,13 +3256,16 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="31.5">
+    <row r="17" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>199</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>217</v>
       </c>
+      <c r="C17" s="2">
+        <v>3357</v>
+      </c>
       <c r="D17" t="s">
         <v>33</v>
       </c>
@@ -3176,13 +3276,16 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="31.5">
+    <row r="18" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>201</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>218</v>
       </c>
+      <c r="C18" s="2">
+        <v>2368</v>
+      </c>
       <c r="D18" t="s">
         <v>33</v>
       </c>
@@ -3193,13 +3296,16 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="31.5">
+    <row r="19" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>209</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>219</v>
       </c>
+      <c r="C19" s="2">
+        <v>5901</v>
+      </c>
       <c r="D19" t="s">
         <v>50</v>
       </c>
@@ -3210,14 +3316,14 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="31.5">
+    <row r="20" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>63</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="2">
         <v>1654</v>
       </c>
       <c r="D20" t="s">
@@ -3230,13 +3336,16 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="31.5">
+    <row r="21" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>211</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>220</v>
       </c>
+      <c r="C21" s="2">
+        <v>2419</v>
+      </c>
       <c r="D21" t="s">
         <v>51</v>
       </c>
@@ -3247,14 +3356,14 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="31.5">
+    <row r="22" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>85</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="2">
         <v>1541</v>
       </c>
       <c r="D22" t="s">
@@ -3285,20 +3394,20 @@
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection sqref="A1:XFD1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.33203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="61.83203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" customWidth="1"/>
-    <col min="4" max="4" width="32.33203125" customWidth="1"/>
-    <col min="5" max="5" width="22.33203125" customWidth="1"/>
+    <col min="1" max="1" width="33.375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="61.875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="10.875" customWidth="1"/>
+    <col min="4" max="4" width="32.375" customWidth="1"/>
+    <col min="5" max="5" width="22.375" customWidth="1"/>
     <col min="6" max="6" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="17.25">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3318,13 +3427,16 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>221</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>222</v>
       </c>
+      <c r="C2" s="2">
+        <v>1098</v>
+      </c>
       <c r="D2" t="s">
         <v>33</v>
       </c>
@@ -3335,13 +3447,16 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="31.5">
+    <row r="3" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>223</v>
       </c>
+      <c r="C3" s="2">
+        <v>2898</v>
+      </c>
       <c r="D3" t="s">
         <v>29</v>
       </c>
@@ -3352,7 +3467,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="31.5">
+    <row r="4" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>224</v>
       </c>
@@ -3370,13 +3485,16 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>226</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>227</v>
       </c>
+      <c r="C5" s="2">
+        <v>65189</v>
+      </c>
       <c r="D5" t="s">
         <v>29</v>
       </c>
@@ -3387,7 +3505,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -3407,7 +3525,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>63</v>
       </c>
@@ -3427,7 +3545,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>64</v>
       </c>
@@ -3447,13 +3565,16 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="31.5">
+    <row r="9" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>228</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>229</v>
       </c>
+      <c r="C9">
+        <v>5544</v>
+      </c>
       <c r="D9" t="s">
         <v>51</v>
       </c>
@@ -3464,13 +3585,16 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="31.5">
+    <row r="10" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>213</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>230</v>
       </c>
+      <c r="C10">
+        <v>13674</v>
+      </c>
       <c r="D10" t="s">
         <v>29</v>
       </c>
@@ -3481,7 +3605,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>231</v>
       </c>
@@ -3493,13 +3617,16 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="31.5">
+    <row r="12" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>221</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>232</v>
       </c>
+      <c r="C12">
+        <v>3394</v>
+      </c>
       <c r="D12" t="s">
         <v>33</v>
       </c>
@@ -3510,13 +3637,16 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="31.5">
+    <row r="13" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>72</v>
       </c>
+      <c r="C13">
+        <v>2840</v>
+      </c>
       <c r="D13" t="s">
         <v>29</v>
       </c>
@@ -3527,7 +3657,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="31.5">
+    <row r="14" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>63</v>
       </c>
@@ -3547,12 +3677,15 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="31.5">
+    <row r="15" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>228</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>233</v>
+      </c>
+      <c r="C15">
+        <v>2856</v>
       </c>
       <c r="D15" t="s">
         <v>51</v>
@@ -3582,19 +3715,19 @@
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection sqref="A1:XFD1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43" customWidth="1"/>
-    <col min="2" max="2" width="73.83203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="24.6640625" customWidth="1"/>
-    <col min="5" max="5" width="21.1640625" customWidth="1"/>
-    <col min="6" max="6" width="19.1640625" customWidth="1"/>
+    <col min="1" max="1" width="38.625" customWidth="1"/>
+    <col min="2" max="2" width="73.875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="24.625" customWidth="1"/>
+    <col min="5" max="5" width="21.125" customWidth="1"/>
+    <col min="6" max="6" width="19.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="17.25">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3614,13 +3747,16 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>234</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>235</v>
       </c>
+      <c r="C2">
+        <v>5824</v>
+      </c>
       <c r="D2" t="s">
         <v>33</v>
       </c>
@@ -3631,13 +3767,16 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>236</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>237</v>
       </c>
+      <c r="C3">
+        <v>4065</v>
+      </c>
       <c r="D3" t="s">
         <v>33</v>
       </c>
@@ -3648,7 +3787,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>238</v>
       </c>
@@ -3666,7 +3805,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>240</v>
       </c>
@@ -3684,13 +3823,16 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>242</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>243</v>
       </c>
+      <c r="C6">
+        <v>81826</v>
+      </c>
       <c r="D6" t="s">
         <v>29</v>
       </c>
@@ -3701,7 +3843,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>63</v>
       </c>
@@ -3721,7 +3863,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>64</v>
       </c>
@@ -3741,7 +3883,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>85</v>
       </c>
@@ -3761,13 +3903,16 @@
         <v>84</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="31.5">
+    <row r="10" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>213</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>214</v>
       </c>
+      <c r="C10">
+        <v>13674</v>
+      </c>
       <c r="D10" t="s">
         <v>29</v>
       </c>
@@ -3778,7 +3923,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>244</v>
       </c>
@@ -3790,13 +3935,16 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>234</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>245</v>
       </c>
+      <c r="C12">
+        <v>2434</v>
+      </c>
       <c r="D12" t="s">
         <v>33</v>
       </c>
@@ -3807,13 +3955,16 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>236</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>246</v>
       </c>
+      <c r="C13">
+        <v>1055</v>
+      </c>
       <c r="D13" t="s">
         <v>33</v>
       </c>
@@ -3824,7 +3975,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>63</v>
       </c>
@@ -3844,7 +3995,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>85</v>
       </c>
@@ -3877,24 +4028,24 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection sqref="A1:XFD1"/>
-      <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
+      <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.5" customWidth="1"/>
-    <col min="2" max="2" width="66.6640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="24.1640625" customWidth="1"/>
-    <col min="5" max="5" width="22.6640625" customWidth="1"/>
+    <col min="1" max="1" width="47.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="66.625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="24.125" customWidth="1"/>
+    <col min="5" max="5" width="22.625" customWidth="1"/>
     <col min="6" max="6" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="17.25">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3914,13 +4065,16 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>247</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>248</v>
       </c>
+      <c r="C2">
+        <v>4127</v>
+      </c>
       <c r="D2" t="s">
         <v>33</v>
       </c>
@@ -3931,13 +4085,16 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>249</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>250</v>
       </c>
+      <c r="C3">
+        <v>4393</v>
+      </c>
       <c r="D3" t="s">
         <v>33</v>
       </c>
@@ -3948,13 +4105,16 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="30">
+    <row r="4" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>251</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>252</v>
       </c>
+      <c r="C4">
+        <v>4411</v>
+      </c>
       <c r="D4" t="s">
         <v>33</v>
       </c>
@@ -3965,30 +4125,34 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="30">
-      <c r="A5" t="s">
+    <row r="5" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="D5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E5" t="s">
-        <v>37</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="C5" s="11"/>
+      <c r="D5" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="11" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>253</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>254</v>
       </c>
+      <c r="C6">
+        <v>65188</v>
+      </c>
       <c r="D6" t="s">
         <v>29</v>
       </c>
@@ -3999,7 +4163,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="30">
+    <row r="7" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>255</v>
       </c>
@@ -4017,13 +4181,16 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>257</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>258</v>
       </c>
+      <c r="C8">
+        <v>461886</v>
+      </c>
       <c r="D8" t="s">
         <v>29</v>
       </c>
@@ -4034,13 +4201,16 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>259</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>260</v>
       </c>
+      <c r="C9">
+        <v>15646</v>
+      </c>
       <c r="D9" t="s">
         <v>29</v>
       </c>
@@ -4051,13 +4221,16 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>261</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>262</v>
       </c>
+      <c r="C10">
+        <v>13426</v>
+      </c>
       <c r="D10" t="s">
         <v>29</v>
       </c>
@@ -4068,13 +4241,16 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="30">
+    <row r="11" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>263</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>264</v>
       </c>
+      <c r="C11">
+        <v>283901</v>
+      </c>
       <c r="D11" t="s">
         <v>29</v>
       </c>
@@ -4085,7 +4261,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>5</v>
       </c>
@@ -4105,13 +4281,16 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>265</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>266</v>
       </c>
+      <c r="C13">
+        <v>479707</v>
+      </c>
       <c r="D13" t="s">
         <v>29</v>
       </c>
@@ -4122,13 +4301,16 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>267</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>268</v>
       </c>
+      <c r="C14">
+        <v>4694</v>
+      </c>
       <c r="D14" t="s">
         <v>50</v>
       </c>
@@ -4139,7 +4321,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="30">
+    <row r="15" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>269</v>
       </c>
@@ -4157,7 +4339,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>271</v>
       </c>
@@ -4175,14 +4357,16 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="30">
+    <row r="17" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>273</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="C17" s="9"/>
+      <c r="C17" s="9">
+        <v>13803</v>
+      </c>
       <c r="D17" t="s">
         <v>29</v>
       </c>
@@ -4193,7 +4377,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>64</v>
       </c>
@@ -4213,13 +4397,16 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>275</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>276</v>
       </c>
+      <c r="C19">
+        <v>14381</v>
+      </c>
       <c r="D19" t="s">
         <v>29</v>
       </c>
@@ -4230,88 +4417,93 @@
         <v>41</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
-      <c r="A33" t="s">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B21" s="12" t="s">
         <v>277</v>
       </c>
-      <c r="D33" t="s">
-        <v>33</v>
-      </c>
-      <c r="E33" t="s">
-        <v>37</v>
-      </c>
-      <c r="F33" t="s">
+      <c r="C21" s="11"/>
+      <c r="D21" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="F21" s="11" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="30">
-      <c r="A34" t="s">
+    <row r="22" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A22" s="11" t="s">
         <v>249</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B22" s="12" t="s">
         <v>278</v>
       </c>
-      <c r="D34" t="s">
-        <v>33</v>
-      </c>
-      <c r="E34" t="s">
-        <v>37</v>
-      </c>
-      <c r="F34" t="s">
+      <c r="C22" s="11"/>
+      <c r="D22" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="F22" s="11" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="30">
-      <c r="A35" t="s">
+    <row r="23" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A23" s="11" t="s">
         <v>251</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B23" s="12" t="s">
         <v>279</v>
       </c>
-      <c r="D35" t="s">
-        <v>33</v>
-      </c>
-      <c r="E35" t="s">
-        <v>37</v>
-      </c>
-      <c r="F35" t="s">
+      <c r="C23" s="11"/>
+      <c r="D23" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="F23" s="11" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="30">
-      <c r="A36" t="s">
+    <row r="24" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A24" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B24" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="D36" t="s">
-        <v>29</v>
-      </c>
-      <c r="E36" t="s">
-        <v>37</v>
-      </c>
-      <c r="F36" t="s">
+      <c r="C24" s="11"/>
+      <c r="D24" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="F24" s="11" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="30">
-      <c r="A37" t="s">
+    <row r="25" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A25" s="11" t="s">
         <v>267</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B25" s="12" t="s">
         <v>280</v>
       </c>
-      <c r="D37" t="s">
+      <c r="C25" s="11"/>
+      <c r="D25" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E25" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="F37" t="s">
+      <c r="F25" s="11" t="s">
         <v>40</v>
       </c>
     </row>
@@ -4332,22 +4524,22 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="46.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="91.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="94.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="46.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="91.125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.75" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.25" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="94.25" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="11" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="17.25">
+    <row r="1" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4367,7 +4559,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>31</v>
       </c>
@@ -4387,7 +4579,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>32</v>
       </c>
@@ -4407,7 +4599,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="7" customFormat="1" ht="31.5">
+    <row r="4" spans="1:7" s="7" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
@@ -4430,7 +4622,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -4450,7 +4642,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>42</v>
       </c>
@@ -4468,7 +4660,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
@@ -4486,7 +4678,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
@@ -4506,7 +4698,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
@@ -4526,7 +4718,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>47</v>
       </c>
@@ -4546,7 +4738,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>7</v>
       </c>
@@ -4564,7 +4756,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>8</v>
       </c>
@@ -4582,7 +4774,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>9</v>
       </c>
@@ -4600,7 +4792,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>10</v>
       </c>
@@ -4618,7 +4810,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>11</v>
       </c>
@@ -4638,7 +4830,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>52</v>
       </c>
@@ -4658,7 +4850,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>12</v>
       </c>
@@ -4676,7 +4868,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>13</v>
       </c>
@@ -4694,7 +4886,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>14</v>
       </c>
@@ -4714,7 +4906,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:6" s="7" customFormat="1">
+    <row r="20" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>2</v>
       </c>
@@ -4734,7 +4926,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>31</v>
       </c>
@@ -4754,7 +4946,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>32</v>
       </c>
@@ -4774,7 +4966,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>47</v>
       </c>
@@ -4794,7 +4986,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>52</v>
       </c>
@@ -4831,20 +5023,20 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2:C12"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="73.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="17.25">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4864,7 +5056,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>55</v>
       </c>
@@ -4884,7 +5076,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="31.5">
+    <row r="3" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -4904,7 +5096,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>60</v>
       </c>
@@ -4922,7 +5114,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -4942,7 +5134,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>63</v>
       </c>
@@ -4962,7 +5154,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>64</v>
       </c>
@@ -4982,7 +5174,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>85</v>
       </c>
@@ -5002,7 +5194,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>58</v>
       </c>
@@ -5022,7 +5214,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="31.5">
+    <row r="10" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -5042,7 +5234,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>63</v>
       </c>
@@ -5062,7 +5254,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>85</v>
       </c>
@@ -5102,16 +5294,16 @@
       <selection pane="bottomLeft" activeCell="C2" sqref="C2:C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.33203125" customWidth="1"/>
+    <col min="1" max="1" width="38.375" customWidth="1"/>
     <col min="2" max="2" width="72.5" style="2" customWidth="1"/>
-    <col min="4" max="4" width="25.33203125" customWidth="1"/>
-    <col min="5" max="5" width="25.1640625" customWidth="1"/>
+    <col min="4" max="4" width="25.375" customWidth="1"/>
+    <col min="5" max="5" width="25.125" customWidth="1"/>
     <col min="6" max="6" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="17.25">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5131,7 +5323,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>73</v>
       </c>
@@ -5151,7 +5343,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="31.5">
+    <row r="3" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>76</v>
       </c>
@@ -5169,7 +5361,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>78</v>
       </c>
@@ -5189,7 +5381,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -5209,7 +5401,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>80</v>
       </c>
@@ -5229,7 +5421,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>64</v>
       </c>
@@ -5249,7 +5441,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>85</v>
       </c>
@@ -5269,7 +5461,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>87</v>
       </c>
@@ -5281,7 +5473,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>73</v>
       </c>
@@ -5301,7 +5493,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>80</v>
       </c>
@@ -5321,7 +5513,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>85</v>
       </c>
@@ -5361,15 +5553,15 @@
       <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39.5" customWidth="1"/>
-    <col min="2" max="2" width="82.6640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="27.1640625" customWidth="1"/>
-    <col min="5" max="6" width="23.83203125" customWidth="1"/>
+    <col min="2" max="2" width="82.625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="27.125" customWidth="1"/>
+    <col min="5" max="6" width="23.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="17.25">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5389,7 +5581,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>88</v>
       </c>
@@ -5409,7 +5601,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>91</v>
       </c>
@@ -5427,7 +5619,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -5447,7 +5639,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>63</v>
       </c>
@@ -5467,7 +5659,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>64</v>
       </c>
@@ -5487,7 +5679,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>85</v>
       </c>
@@ -5507,7 +5699,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>88</v>
       </c>
@@ -5527,7 +5719,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>63</v>
       </c>
@@ -5547,7 +5739,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>85</v>
       </c>

</xml_diff>

<commit_message>
Updated GI Carcinoid Tumors and Breast Cancer; Also added Carcinoma of Unknown Primary and Cervical Cancer.
</commit_message>
<xml_diff>
--- a/Daisy-xls/IA/CTHP-Cards.xlsx
+++ b/Daisy-xls/IA/CTHP-Cards.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-495" windowWidth="28860" windowHeight="16545" tabRatio="655" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="655" firstSheet="5" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="BRAIN" sheetId="6" r:id="rId1"/>
@@ -17,6 +17,8 @@
     <sheet name="ANAL" sheetId="3" r:id="rId8"/>
     <sheet name="GI CARCINOID TUMOR" sheetId="4" r:id="rId9"/>
     <sheet name="LEUKEMIA" sheetId="5" r:id="rId10"/>
+    <sheet name="CARCINOMA OF UNKNOWN PRIMARY" sheetId="11" r:id="rId11"/>
+    <sheet name="CERVICAL" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1034" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1250" uniqueCount="334">
   <si>
     <t>Title</t>
   </si>
@@ -871,6 +873,165 @@
   </si>
   <si>
     <t>http://www.cancer.gov/cancertopics/pdq/prevention/breast/HealthProfessional</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/factsheet/Risk/reproductive-history</t>
+  </si>
+  <si>
+    <t>Reproductive History and Breast Cancer Risk</t>
+  </si>
+  <si>
+    <t>BRCA1and BRCA2: Cancer Risk and Genetic Testing</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/factsheet/Risk/BRCA</t>
+  </si>
+  <si>
+    <t>Genetics of Breast and Gynecologic Cancers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PDQ Genetics Information </t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/pdq/genetics/breast-and-ovarian/HealthProfessional</t>
+  </si>
+  <si>
+    <t>Genetics</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/pdq/screening/breast/Patient</t>
+  </si>
+  <si>
+    <t>Breast Cancer Screening</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/pdq/screening/breast/healthprofessional</t>
+  </si>
+  <si>
+    <t>Mammograms</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/factsheet/detection/mammograms</t>
+  </si>
+  <si>
+    <t>Find an FDA Certified Mammogram Facility</t>
+  </si>
+  <si>
+    <t>http://www.accessdata.fda.gov/scripts/cdrh/cfdocs/cfMQSA/mqsa.cfm</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/clinicaltrials/search/results?protocolsearchid=6175345&amp;vers=1</t>
+  </si>
+  <si>
+    <t>Clinical Trials to Screen for Breast Cancer</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/types/breast/beyond-cancer-video</t>
+  </si>
+  <si>
+    <t>Moving Beyond Breast Cancer Videos</t>
+  </si>
+  <si>
+    <t>General Resources on Coping</t>
+  </si>
+  <si>
+    <t>Coping</t>
+  </si>
+  <si>
+    <t>http://seer.cancer.gov/statfacts/html/breast.html</t>
+  </si>
+  <si>
+    <t>http://seer.cancer.gov/statfacts/html/lungb.html</t>
+  </si>
+  <si>
+    <t>Carcinoma of Unknown Primary Treatment</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/pdq/treatment/unknownprimary/Patient</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/pdq/treatment/unknownprimary/HealthProfessional</t>
+  </si>
+  <si>
+    <t>Clinical Trials to Treat Carcinoma of Unknown Primary</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/clinicaltrials/search/results?protocolsearchid=8167069&amp;vers=1</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/pdq/treatment/cervical/Patient</t>
+  </si>
+  <si>
+    <t>Cervical Cancer Treatment</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/pdq/treatment/cervical/HealthProfessional</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/clinicaltrials/search/results?protocolsearchid=8693745&amp;vers=1</t>
+  </si>
+  <si>
+    <t>Clinical Trials to Treat Cervical Cancer</t>
+  </si>
+  <si>
+    <t>Drugs Approved for Cervical Cancer</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/druginfo/cervicalcancer</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/pdq/prevention/cervical/Patient</t>
+  </si>
+  <si>
+    <t>Cervical Cancer Prevention</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/pdq/prevention/cervical/HealthProfessional</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/clinicaltrials/search/results?protocolsearchid=6197728&amp;vers=1</t>
+  </si>
+  <si>
+    <t>Clinical Trials to Prevent Cervical Cancer</t>
+  </si>
+  <si>
+    <t>Infectious Agents</t>
+  </si>
+  <si>
+    <t>DOES NOT EXIST YET</t>
+  </si>
+  <si>
+    <t>Cervical Cancer Screening</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/pdq/screening/cervical/Patient</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/pdq/screening/cervical/HealthProfessional</t>
+  </si>
+  <si>
+    <t>Understanding Cervical Changes: A Health Guide for Women</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/understanding-cervical-changes</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/factsheet/detection/Pap-HPV-testing</t>
+  </si>
+  <si>
+    <t>Pap and HPV Testing</t>
+  </si>
+  <si>
+    <t>National Breast and Cervical Cancer Early Detection Program (NBCCEDP)</t>
+  </si>
+  <si>
+    <t>Clinical Trials to Screen for Cervical Cancer</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/clinicaltrials/search/results?protocolsearchid=6124856&amp;vers=1</t>
+  </si>
+  <si>
+    <t>http://seer.cancer.gov/statfacts/html/cervix.html</t>
   </si>
 </sst>
 </file>
@@ -909,7 +1070,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -934,6 +1095,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF79646"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -944,7 +1111,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="80">
+  <cellStyleXfs count="126">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1025,8 +1192,54 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1054,8 +1267,13 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="80">
+  <cellStyles count="126">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1118,6 +1336,29 @@
     <cellStyle name="Followed Hyperlink" xfId="77" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="79" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="81" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="83" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="85" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="87" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="89" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="91" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="93" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="95" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="97" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="99" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="101" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="103" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="105" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="107" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="109" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="111" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="113" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="115" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="117" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="119" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="121" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="123" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="125" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1135,6 +1376,29 @@
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="80" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="82" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="84" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="86" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="88" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="90" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="92" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="94" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="96" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="98" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="100" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="102" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="104" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="106" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="108" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="110" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="112" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="114" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="116" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="118" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="120" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="122" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="124" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1471,22 +1735,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection sqref="A1:XFD1"/>
       <selection pane="bottomLeft" activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="56.125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="56.1640625" style="2" customWidth="1"/>
     <col min="2" max="2" width="47.5" style="2" customWidth="1"/>
-    <col min="4" max="4" width="26.125" customWidth="1"/>
-    <col min="5" max="5" width="22.375" customWidth="1"/>
-    <col min="6" max="6" width="19.375" customWidth="1"/>
+    <col min="4" max="4" width="26.1640625" customWidth="1"/>
+    <col min="5" max="5" width="22.33203125" customWidth="1"/>
+    <col min="6" max="6" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="17.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1506,7 +1770,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="31.5">
       <c r="A2" s="2" t="s">
         <v>139</v>
       </c>
@@ -1526,7 +1790,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="31.5">
       <c r="A3" s="2" t="s">
         <v>141</v>
       </c>
@@ -1546,7 +1810,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="31.5">
       <c r="A4" s="2" t="s">
         <v>143</v>
       </c>
@@ -1566,7 +1830,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="31.5">
       <c r="A5" s="2" t="s">
         <v>145</v>
       </c>
@@ -1586,7 +1850,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="31.5">
       <c r="A6" s="2" t="s">
         <v>147</v>
       </c>
@@ -1606,7 +1870,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="31.5">
       <c r="A7" s="2" t="s">
         <v>149</v>
       </c>
@@ -1626,7 +1890,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="31.5">
       <c r="A8" s="2" t="s">
         <v>151</v>
       </c>
@@ -1646,7 +1910,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="31.5">
       <c r="A9" s="2" t="s">
         <v>153</v>
       </c>
@@ -1666,7 +1930,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="31.5">
       <c r="A10" s="2" t="s">
         <v>155</v>
       </c>
@@ -1686,7 +1950,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="31.5">
       <c r="A11" s="2" t="s">
         <v>157</v>
       </c>
@@ -1706,7 +1970,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="31.5">
       <c r="A12" s="2" t="s">
         <v>159</v>
       </c>
@@ -1726,7 +1990,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" s="2" t="s">
         <v>162</v>
       </c>
@@ -1744,7 +2008,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="31.5">
       <c r="A14" s="2" t="s">
         <v>164</v>
       </c>
@@ -1762,7 +2026,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="31.5">
       <c r="A15" s="2" t="s">
         <v>166</v>
       </c>
@@ -1780,7 +2044,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="31.5">
       <c r="A16" s="2" t="s">
         <v>168</v>
       </c>
@@ -1798,7 +2062,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="31.5">
       <c r="A17" s="2" t="s">
         <v>170</v>
       </c>
@@ -1816,7 +2080,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="31.5">
       <c r="A18" s="2" t="s">
         <v>172</v>
       </c>
@@ -1834,7 +2098,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="31.5">
       <c r="A19" s="2" t="s">
         <v>174</v>
       </c>
@@ -1852,7 +2116,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="31.5">
       <c r="A20" s="2" t="s">
         <v>176</v>
       </c>
@@ -1870,7 +2134,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="31.5">
       <c r="A21" s="2" t="s">
         <v>178</v>
       </c>
@@ -1888,7 +2152,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="31.5">
       <c r="A22" s="2" t="s">
         <v>180</v>
       </c>
@@ -1906,7 +2170,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="31.5">
       <c r="A23" s="2" t="s">
         <v>182</v>
       </c>
@@ -1924,7 +2188,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="31.5">
       <c r="A24" s="2" t="s">
         <v>184</v>
       </c>
@@ -1942,7 +2206,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="31.5">
       <c r="A25" s="6" t="s">
         <v>63</v>
       </c>
@@ -1962,7 +2226,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="31.5">
       <c r="A26" s="6" t="s">
         <v>64</v>
       </c>
@@ -1982,7 +2246,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="31.5">
       <c r="A27" s="6" t="s">
         <v>85</v>
       </c>
@@ -2002,7 +2266,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6">
       <c r="B28" s="2" t="s">
         <v>186</v>
       </c>
@@ -2014,7 +2278,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="31.5">
       <c r="A29" s="2" t="s">
         <v>139</v>
       </c>
@@ -2034,7 +2298,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="31.5">
       <c r="A30" s="2" t="s">
         <v>141</v>
       </c>
@@ -2054,7 +2318,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="31.5">
       <c r="A31" s="2" t="s">
         <v>143</v>
       </c>
@@ -2074,7 +2338,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="31.5">
       <c r="A32" s="2" t="s">
         <v>145</v>
       </c>
@@ -2094,7 +2358,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="31.5">
       <c r="A33" s="2" t="s">
         <v>147</v>
       </c>
@@ -2114,7 +2378,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="31.5">
       <c r="A34" s="2" t="s">
         <v>149</v>
       </c>
@@ -2134,7 +2398,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="31.5">
       <c r="A35" s="2" t="s">
         <v>151</v>
       </c>
@@ -2154,7 +2418,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="31.5">
       <c r="A36" s="2" t="s">
         <v>153</v>
       </c>
@@ -2174,7 +2438,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" ht="31.5">
       <c r="A37" s="2" t="s">
         <v>155</v>
       </c>
@@ -2194,7 +2458,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" ht="31.5">
       <c r="A38" s="2" t="s">
         <v>157</v>
       </c>
@@ -2214,7 +2478,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" ht="31.5">
       <c r="A39" t="s">
         <v>63</v>
       </c>
@@ -2234,7 +2498,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" ht="31.5">
       <c r="A40" t="s">
         <v>85</v>
       </c>
@@ -2269,20 +2533,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2:C31"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="46" style="2" customWidth="1"/>
-    <col min="2" max="2" width="69.375" style="2" customWidth="1"/>
-    <col min="4" max="5" width="24.625" customWidth="1"/>
-    <col min="6" max="6" width="18.375" customWidth="1"/>
+    <col min="2" max="2" width="69.33203125" style="2" customWidth="1"/>
+    <col min="4" max="5" width="24.6640625" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="17.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2302,7 +2566,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
         <v>94</v>
       </c>
@@ -2322,7 +2586,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="2" t="s">
         <v>96</v>
       </c>
@@ -2342,7 +2606,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="2" t="s">
         <v>99</v>
       </c>
@@ -2362,7 +2626,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="31.5">
       <c r="A5" s="2" t="s">
         <v>102</v>
       </c>
@@ -2382,7 +2646,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="2" t="s">
         <v>105</v>
       </c>
@@ -2402,7 +2666,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" s="2" t="s">
         <v>108</v>
       </c>
@@ -2422,7 +2686,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" s="2" t="s">
         <v>111</v>
       </c>
@@ -2442,7 +2706,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" s="2" t="s">
         <v>116</v>
       </c>
@@ -2462,7 +2726,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="31.5">
       <c r="A10" s="2" t="s">
         <v>119</v>
       </c>
@@ -2480,7 +2744,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="31.5">
       <c r="A11" s="2" t="s">
         <v>120</v>
       </c>
@@ -2498,7 +2762,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="31.5">
       <c r="A12" s="2" t="s">
         <v>122</v>
       </c>
@@ -2516,7 +2780,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="31.5">
       <c r="A13" s="2" t="s">
         <v>124</v>
       </c>
@@ -2534,7 +2798,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="31.5">
       <c r="A14" s="2" t="s">
         <v>130</v>
       </c>
@@ -2552,7 +2816,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="31.5">
       <c r="A15" s="2" t="s">
         <v>128</v>
       </c>
@@ -2570,7 +2834,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="31.5">
       <c r="A16" s="2" t="s">
         <v>126</v>
       </c>
@@ -2588,7 +2852,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="31.5">
       <c r="A17" s="2" t="s">
         <v>132</v>
       </c>
@@ -2606,7 +2870,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="31.5">
       <c r="A18" s="2" t="s">
         <v>134</v>
       </c>
@@ -2624,7 +2888,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="31.5">
       <c r="A19" s="2" t="s">
         <v>135</v>
       </c>
@@ -2642,7 +2906,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6">
       <c r="A20" s="6" t="s">
         <v>63</v>
       </c>
@@ -2662,7 +2926,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6">
       <c r="A21" s="6" t="s">
         <v>64</v>
       </c>
@@ -2682,7 +2946,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6">
       <c r="A22" s="6" t="s">
         <v>85</v>
       </c>
@@ -2702,7 +2966,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6">
       <c r="A23" s="6"/>
       <c r="B23" s="2" t="s">
         <v>138</v>
@@ -2715,7 +2979,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6">
       <c r="A24" s="2" t="s">
         <v>94</v>
       </c>
@@ -2735,7 +2999,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6">
       <c r="A25" s="2" t="s">
         <v>96</v>
       </c>
@@ -2755,7 +3019,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6">
       <c r="A26" s="2" t="s">
         <v>99</v>
       </c>
@@ -2775,7 +3039,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="31.5">
       <c r="A27" s="2" t="s">
         <v>102</v>
       </c>
@@ -2795,7 +3059,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6">
       <c r="A28" s="2" t="s">
         <v>105</v>
       </c>
@@ -2815,7 +3079,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6">
       <c r="A29" s="2" t="s">
         <v>108</v>
       </c>
@@ -2835,7 +3099,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="31.5">
       <c r="A30" s="2" t="s">
         <v>111</v>
       </c>
@@ -2855,7 +3119,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6">
       <c r="A31" s="2" t="s">
         <v>115</v>
       </c>
@@ -2875,7 +3139,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="31.5">
       <c r="A32" t="s">
         <v>63</v>
       </c>
@@ -2895,7 +3159,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6">
       <c r="A33" t="s">
         <v>85</v>
       </c>
@@ -2912,6 +3176,634 @@
         <v>44</v>
       </c>
       <c r="F33" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="43.5" customWidth="1"/>
+    <col min="2" max="2" width="72.5" style="2" customWidth="1"/>
+    <col min="4" max="4" width="27.33203125" customWidth="1"/>
+    <col min="5" max="5" width="18.83203125" customWidth="1"/>
+    <col min="6" max="6" width="16.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="16">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="13" t="s">
+        <v>304</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>305</v>
+      </c>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="30">
+      <c r="A3" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>307</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C5">
+        <v>6158</v>
+      </c>
+      <c r="D5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6">
+        <v>899999</v>
+      </c>
+      <c r="D6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7">
+        <v>6145</v>
+      </c>
+      <c r="D7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="30">
+      <c r="A8" s="13" t="s">
+        <v>304</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>306</v>
+      </c>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="30">
+      <c r="A9" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10">
+        <v>1654</v>
+      </c>
+      <c r="D10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>85</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11">
+        <v>1541</v>
+      </c>
+      <c r="D11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="42.33203125" customWidth="1"/>
+    <col min="2" max="2" width="62" style="2" customWidth="1"/>
+    <col min="4" max="4" width="23.83203125" customWidth="1"/>
+    <col min="5" max="5" width="22.5" customWidth="1"/>
+    <col min="6" max="6" width="16" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="16">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="13" t="s">
+        <v>310</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="30">
+      <c r="A3" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="30">
+      <c r="A4" t="s">
+        <v>313</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="13" t="s">
+        <v>314</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>315</v>
+      </c>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="2">
+        <v>6835</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="13" t="s">
+        <v>317</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>316</v>
+      </c>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="30">
+      <c r="A8" t="s">
+        <v>320</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9">
+        <v>899999</v>
+      </c>
+      <c r="D9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="6" t="s">
+        <v>321</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="D10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="15" t="s">
+        <v>323</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>324</v>
+      </c>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="15" t="s">
+        <v>326</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>327</v>
+      </c>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="30">
+      <c r="A13" s="15" t="s">
+        <v>329</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>328</v>
+      </c>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="30">
+      <c r="A14" s="6" t="s">
+        <v>330</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="C14" s="5"/>
+      <c r="D14" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="30">
+      <c r="A15" s="6" t="s">
+        <v>331</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="C15" s="5"/>
+      <c r="D15" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="6"/>
+      <c r="B16" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="C16" s="5"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="30">
+      <c r="A17" s="13" t="s">
+        <v>310</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>311</v>
+      </c>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="30">
+      <c r="A18" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="30">
+      <c r="A19" s="13" t="s">
+        <v>317</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>318</v>
+      </c>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="F19" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="30">
+      <c r="A20" s="13" t="s">
+        <v>323</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>325</v>
+      </c>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="F20" s="13" t="s">
         <v>40</v>
       </c>
     </row>
@@ -2936,16 +3828,16 @@
       <selection pane="bottomLeft" activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="40.375" customWidth="1"/>
-    <col min="2" max="2" width="59.875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="40.33203125" customWidth="1"/>
+    <col min="2" max="2" width="59.83203125" style="2" customWidth="1"/>
     <col min="4" max="4" width="24" customWidth="1"/>
-    <col min="5" max="5" width="23.375" customWidth="1"/>
-    <col min="6" max="6" width="19.375" customWidth="1"/>
+    <col min="5" max="5" width="23.33203125" customWidth="1"/>
+    <col min="6" max="6" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="17.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2965,7 +3857,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>197</v>
       </c>
@@ -2985,7 +3877,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="31.5">
       <c r="A3" t="s">
         <v>199</v>
       </c>
@@ -3005,7 +3897,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>201</v>
       </c>
@@ -3025,7 +3917,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="31.5">
       <c r="A5" t="s">
         <v>203</v>
       </c>
@@ -3043,7 +3935,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>205</v>
       </c>
@@ -3063,7 +3955,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>207</v>
       </c>
@@ -3083,7 +3975,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
@@ -3103,7 +3995,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="31.5">
       <c r="A9" s="2" t="s">
         <v>209</v>
       </c>
@@ -3123,7 +4015,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" s="6" t="s">
         <v>63</v>
       </c>
@@ -3143,7 +4035,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="31.5">
       <c r="A11" s="6" t="s">
         <v>64</v>
       </c>
@@ -3163,7 +4055,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="31.5">
       <c r="A12" s="6" t="s">
         <v>211</v>
       </c>
@@ -3183,7 +4075,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" s="6" t="s">
         <v>85</v>
       </c>
@@ -3203,7 +4095,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="31.5">
       <c r="A14" s="6" t="s">
         <v>213</v>
       </c>
@@ -3223,7 +4115,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="A15" s="6"/>
       <c r="B15" s="2" t="s">
         <v>215</v>
@@ -3236,7 +4128,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="31.5">
       <c r="A16" t="s">
         <v>197</v>
       </c>
@@ -3256,7 +4148,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="31.5">
       <c r="A17" t="s">
         <v>199</v>
       </c>
@@ -3276,7 +4168,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="31.5">
       <c r="A18" t="s">
         <v>201</v>
       </c>
@@ -3296,7 +4188,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="31.5">
       <c r="A19" t="s">
         <v>209</v>
       </c>
@@ -3316,7 +4208,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="31.5">
       <c r="A20" t="s">
         <v>63</v>
       </c>
@@ -3336,7 +4228,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="31.5">
       <c r="A21" s="6" t="s">
         <v>211</v>
       </c>
@@ -3356,7 +4248,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="31.5">
       <c r="A22" t="s">
         <v>85</v>
       </c>
@@ -3397,17 +4289,17 @@
       <selection pane="bottomLeft" activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="33.375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="61.875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="10.875" customWidth="1"/>
-    <col min="4" max="4" width="32.375" customWidth="1"/>
-    <col min="5" max="5" width="22.375" customWidth="1"/>
+    <col min="1" max="1" width="33.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="61.83203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" customWidth="1"/>
+    <col min="4" max="4" width="32.33203125" customWidth="1"/>
+    <col min="5" max="5" width="22.33203125" customWidth="1"/>
     <col min="6" max="6" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="17.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3427,7 +4319,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
         <v>221</v>
       </c>
@@ -3447,7 +4339,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="31.5">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -3467,7 +4359,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="31.5">
       <c r="A4" s="2" t="s">
         <v>224</v>
       </c>
@@ -3485,7 +4377,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="2" t="s">
         <v>226</v>
       </c>
@@ -3505,7 +4397,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -3525,7 +4417,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" s="10" t="s">
         <v>63</v>
       </c>
@@ -3545,7 +4437,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" s="10" t="s">
         <v>64</v>
       </c>
@@ -3565,7 +4457,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="31.5">
       <c r="A9" s="10" t="s">
         <v>228</v>
       </c>
@@ -3585,7 +4477,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="31.5">
       <c r="A10" s="2" t="s">
         <v>213</v>
       </c>
@@ -3605,7 +4497,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="B11" s="2" t="s">
         <v>231</v>
       </c>
@@ -3617,7 +4509,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="31.5">
       <c r="A12" s="2" t="s">
         <v>221</v>
       </c>
@@ -3637,7 +4529,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="31.5">
       <c r="A13" s="2" t="s">
         <v>2</v>
       </c>
@@ -3657,7 +4549,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="31.5">
       <c r="A14" s="2" t="s">
         <v>63</v>
       </c>
@@ -3677,7 +4569,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="31.5">
       <c r="A15" s="10" t="s">
         <v>228</v>
       </c>
@@ -3718,16 +4610,16 @@
       <selection pane="bottomLeft" activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="38.625" customWidth="1"/>
-    <col min="2" max="2" width="73.875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="24.625" customWidth="1"/>
-    <col min="5" max="5" width="21.125" customWidth="1"/>
-    <col min="6" max="6" width="19.125" customWidth="1"/>
+    <col min="1" max="1" width="38.6640625" customWidth="1"/>
+    <col min="2" max="2" width="73.83203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="24.6640625" customWidth="1"/>
+    <col min="5" max="5" width="21.1640625" customWidth="1"/>
+    <col min="6" max="6" width="19.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="17.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3747,7 +4639,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>234</v>
       </c>
@@ -3767,7 +4659,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>236</v>
       </c>
@@ -3787,7 +4679,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>238</v>
       </c>
@@ -3805,7 +4697,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>240</v>
       </c>
@@ -3823,7 +4715,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>242</v>
       </c>
@@ -3843,7 +4735,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" s="10" t="s">
         <v>63</v>
       </c>
@@ -3863,7 +4755,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" s="10" t="s">
         <v>64</v>
       </c>
@@ -3883,7 +4775,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" s="6" t="s">
         <v>85</v>
       </c>
@@ -3903,7 +4795,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="31.5">
       <c r="A10" s="6" t="s">
         <v>213</v>
       </c>
@@ -3923,7 +4815,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="B11" s="2" t="s">
         <v>244</v>
       </c>
@@ -3935,7 +4827,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>234</v>
       </c>
@@ -3955,7 +4847,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>236</v>
       </c>
@@ -3975,7 +4867,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14" s="2" t="s">
         <v>63</v>
       </c>
@@ -3995,7 +4887,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>85</v>
       </c>
@@ -4028,24 +4920,24 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection sqref="A1:XFD1"/>
-      <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
+      <selection pane="bottomLeft" activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="47.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="66.625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="24.125" customWidth="1"/>
-    <col min="5" max="5" width="22.625" customWidth="1"/>
+    <col min="1" max="1" width="47.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="66.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="24.1640625" customWidth="1"/>
+    <col min="5" max="5" width="22.6640625" customWidth="1"/>
     <col min="6" max="6" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="17.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4065,7 +4957,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>247</v>
       </c>
@@ -4085,7 +4977,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>249</v>
       </c>
@@ -4105,7 +4997,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="31.5">
       <c r="A4" t="s">
         <v>251</v>
       </c>
@@ -4125,7 +5017,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="31.5">
       <c r="A5" s="11" t="s">
         <v>2</v>
       </c>
@@ -4143,7 +5035,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>253</v>
       </c>
@@ -4163,7 +5055,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="31.5">
       <c r="A7" t="s">
         <v>255</v>
       </c>
@@ -4181,7 +5073,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>257</v>
       </c>
@@ -4201,7 +5093,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="31.5">
       <c r="A9" t="s">
         <v>259</v>
       </c>
@@ -4221,7 +5113,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>261</v>
       </c>
@@ -4241,7 +5133,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="31.5">
       <c r="A11" t="s">
         <v>263</v>
       </c>
@@ -4261,7 +5153,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" s="2" t="s">
         <v>5</v>
       </c>
@@ -4281,7 +5173,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>265</v>
       </c>
@@ -4301,7 +5193,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>267</v>
       </c>
@@ -4321,7 +5213,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="31.5">
       <c r="A15" t="s">
         <v>269</v>
       </c>
@@ -4339,7 +5231,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>271</v>
       </c>
@@ -4357,7 +5249,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="31.5">
       <c r="A17" t="s">
         <v>273</v>
       </c>
@@ -4377,7 +5269,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>64</v>
       </c>
@@ -4397,7 +5289,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
         <v>275</v>
       </c>
@@ -4417,93 +5309,266 @@
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="11" t="s">
+    <row r="20" spans="1:6">
+      <c r="A20" s="11" t="s">
+        <v>282</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>281</v>
+      </c>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="13" t="s">
+        <v>290</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>289</v>
+      </c>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="F21" s="13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>293</v>
+      </c>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="F22" s="13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" t="s">
+        <v>294</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="C23" s="5"/>
+      <c r="D23" t="s">
+        <v>29</v>
+      </c>
+      <c r="E23" t="s">
+        <v>44</v>
+      </c>
+      <c r="F23" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="30">
+      <c r="A24" t="s">
+        <v>297</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="C24" s="5"/>
+      <c r="D24" t="s">
+        <v>29</v>
+      </c>
+      <c r="E24" t="s">
+        <v>44</v>
+      </c>
+      <c r="F24" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="13" t="s">
+        <v>299</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>298</v>
+      </c>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13" t="s">
+        <v>300</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>301</v>
+      </c>
+      <c r="F25" s="13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="B26" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="B21" s="12" t="s">
+      <c r="B28" s="12" t="s">
         <v>277</v>
       </c>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11" t="s">
+      <c r="C28" s="11"/>
+      <c r="D28" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="E21" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="F21" s="11" t="s">
+      <c r="E28" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="F28" s="11" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="11" t="s">
+    <row r="29" spans="1:6" ht="31.5">
+      <c r="A29" s="13" t="s">
         <v>249</v>
       </c>
-      <c r="B22" s="12" t="s">
+      <c r="B29" s="12" t="s">
         <v>278</v>
       </c>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11" t="s">
+      <c r="C29" s="11"/>
+      <c r="D29" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="E22" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="F22" s="11" t="s">
+      <c r="E29" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="F29" s="11" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A23" s="11" t="s">
+    <row r="30" spans="1:6" ht="31.5">
+      <c r="A30" s="11" t="s">
         <v>251</v>
       </c>
-      <c r="B23" s="12" t="s">
+      <c r="B30" s="12" t="s">
         <v>279</v>
       </c>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11" t="s">
+      <c r="C30" s="11"/>
+      <c r="D30" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="E23" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="F23" s="11" t="s">
+      <c r="E30" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="F30" s="11" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A24" s="11" t="s">
+    <row r="31" spans="1:6" ht="31.5">
+      <c r="A31" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B24" s="12" t="s">
+      <c r="B31" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="E24" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="F24" s="11" t="s">
+      <c r="C31" s="11"/>
+      <c r="D31" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E31" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="F31" s="11" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A25" s="11" t="s">
+    <row r="32" spans="1:6" ht="31.5">
+      <c r="A32" s="11" t="s">
         <v>267</v>
       </c>
-      <c r="B25" s="12" t="s">
+      <c r="B32" s="12" t="s">
         <v>280</v>
       </c>
-      <c r="C25" s="11"/>
-      <c r="D25" s="11" t="s">
+      <c r="C32" s="11"/>
+      <c r="D32" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="E25" s="11" t="s">
+      <c r="E32" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="F25" s="11" t="s">
+      <c r="F32" s="11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="30">
+      <c r="A33" s="11" t="s">
+        <v>285</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>287</v>
+      </c>
+      <c r="C33" s="13"/>
+      <c r="D33" s="11" t="s">
+        <v>286</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>288</v>
+      </c>
+      <c r="F33" s="11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="13" t="s">
+        <v>283</v>
+      </c>
+      <c r="B34" s="14" t="s">
+        <v>284</v>
+      </c>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E34" s="13" t="s">
+        <v>288</v>
+      </c>
+      <c r="F34" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="11" t="s">
+        <v>290</v>
+      </c>
+      <c r="B35" s="14" t="s">
+        <v>291</v>
+      </c>
+      <c r="C35" s="13"/>
+      <c r="D35" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="E35" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="F35" s="11" t="s">
         <v>40</v>
       </c>
     </row>
@@ -4520,26 +5585,26 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="46.625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="91.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.75" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.25" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.875" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="94.25" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="46.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="91.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="94.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="11" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="17.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4559,7 +5624,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="2" t="s">
         <v>31</v>
       </c>
@@ -4579,7 +5644,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="2" t="s">
         <v>32</v>
       </c>
@@ -4599,7 +5664,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="7" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" s="7" customFormat="1" ht="31.5">
       <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
@@ -4622,7 +5687,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -4642,7 +5707,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="2" t="s">
         <v>42</v>
       </c>
@@ -4660,7 +5725,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
@@ -4678,7 +5743,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
@@ -4698,7 +5763,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
@@ -4718,7 +5783,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="2" t="s">
         <v>47</v>
       </c>
@@ -4738,7 +5803,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="2" t="s">
         <v>7</v>
       </c>
@@ -4756,7 +5821,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="2" t="s">
         <v>8</v>
       </c>
@@ -4774,7 +5839,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" s="2" t="s">
         <v>9</v>
       </c>
@@ -4792,7 +5857,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="A14" s="2" t="s">
         <v>10</v>
       </c>
@@ -4810,7 +5875,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7">
       <c r="A15" s="2" t="s">
         <v>11</v>
       </c>
@@ -4830,7 +5895,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7">
       <c r="A16" s="2" t="s">
         <v>52</v>
       </c>
@@ -4850,7 +5915,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6">
       <c r="A17" s="2" t="s">
         <v>12</v>
       </c>
@@ -4868,7 +5933,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6">
       <c r="A18" s="2" t="s">
         <v>13</v>
       </c>
@@ -4886,7 +5951,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6">
       <c r="A19" s="2" t="s">
         <v>14</v>
       </c>
@@ -4906,55 +5971,47 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
+    <row r="20" spans="1:6" ht="30">
+      <c r="B20" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="C20" s="3"/>
+      <c r="E20" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" s="7" customFormat="1">
+      <c r="A21" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B21" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="C20" s="8">
+      <c r="C21" s="8">
         <v>2840</v>
       </c>
-      <c r="D20" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="F20" s="7" t="s">
+      <c r="D21" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="F21" s="7" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+    <row r="22" spans="1:6">
+      <c r="A22" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B22" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C22" s="2">
         <v>3853</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C22" s="2">
-        <v>4031</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>33</v>
@@ -4966,43 +6023,63 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6">
       <c r="A23" s="2" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C23" s="2">
-        <v>2190</v>
+        <v>4031</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6">
       <c r="A24" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" s="2">
+        <v>2190</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B25" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C25" s="2">
         <v>2301</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D25" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="E25" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="F24" s="2" t="s">
+      <c r="F25" s="2" t="s">
         <v>40</v>
       </c>
     </row>
@@ -5023,20 +6100,20 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5:F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="41" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="73.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="17.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5056,7 +6133,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>55</v>
       </c>
@@ -5076,7 +6153,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="31.5">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -5096,7 +6173,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="4" t="s">
         <v>60</v>
       </c>
@@ -5114,7 +6191,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -5134,7 +6211,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="6" t="s">
         <v>63</v>
       </c>
@@ -5154,7 +6231,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" s="6" t="s">
         <v>64</v>
       </c>
@@ -5174,7 +6251,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" s="6" t="s">
         <v>85</v>
       </c>
@@ -5194,7 +6271,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>58</v>
       </c>
@@ -5214,7 +6291,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="31.5">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -5234,7 +6311,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>63</v>
       </c>
@@ -5254,7 +6331,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>85</v>
       </c>
@@ -5294,16 +6371,16 @@
       <selection pane="bottomLeft" activeCell="C2" sqref="C2:C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="38.375" customWidth="1"/>
+    <col min="1" max="1" width="38.33203125" customWidth="1"/>
     <col min="2" max="2" width="72.5" style="2" customWidth="1"/>
-    <col min="4" max="4" width="25.375" customWidth="1"/>
-    <col min="5" max="5" width="25.125" customWidth="1"/>
+    <col min="4" max="4" width="25.33203125" customWidth="1"/>
+    <col min="5" max="5" width="25.1640625" customWidth="1"/>
     <col min="6" max="6" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="17.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5323,7 +6400,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>73</v>
       </c>
@@ -5343,7 +6420,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="31.5">
       <c r="A3" t="s">
         <v>76</v>
       </c>
@@ -5361,7 +6438,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>78</v>
       </c>
@@ -5381,7 +6458,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -5401,7 +6478,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>80</v>
       </c>
@@ -5421,7 +6498,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" s="6" t="s">
         <v>64</v>
       </c>
@@ -5441,7 +6518,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" s="6" t="s">
         <v>85</v>
       </c>
@@ -5461,7 +6538,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="B9" s="2" t="s">
         <v>87</v>
       </c>
@@ -5473,7 +6550,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>73</v>
       </c>
@@ -5493,7 +6570,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>80</v>
       </c>
@@ -5513,7 +6590,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>85</v>
       </c>
@@ -5546,22 +6623,22 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="39.5" customWidth="1"/>
-    <col min="2" max="2" width="82.625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="27.125" customWidth="1"/>
-    <col min="5" max="6" width="23.875" customWidth="1"/>
+    <col min="2" max="2" width="82.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="27.1640625" customWidth="1"/>
+    <col min="5" max="6" width="23.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="17.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5581,7 +6658,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>88</v>
       </c>
@@ -5601,73 +6678,71 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:6">
+      <c r="A3" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" s="14"/>
+      <c r="D3" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
         <v>91</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B4" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" t="s">
-        <v>37</v>
-      </c>
-      <c r="F3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="C4" s="5"/>
+      <c r="D4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C5" s="2">
         <v>6835</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F4" s="2" t="s">
+      <c r="D5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+    <row r="6" spans="1:6">
+      <c r="A6" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B6" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C5">
+      <c r="C6">
         <v>6158</v>
-      </c>
-      <c r="D5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E5" t="s">
-        <v>43</v>
-      </c>
-      <c r="F5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C6">
-        <v>899999</v>
       </c>
       <c r="D6" t="s">
         <v>29</v>
@@ -5676,86 +6751,124 @@
         <v>43</v>
       </c>
       <c r="F6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7">
+        <v>899999</v>
+      </c>
+      <c r="D7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B8" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C7">
+      <c r="C8">
         <v>6145</v>
       </c>
-      <c r="D7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="D8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" t="s">
         <v>44</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F8" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
         <v>88</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B9" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C9" s="2">
         <v>5003</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D9" t="s">
         <v>33</v>
       </c>
-      <c r="E8" t="s">
-        <v>37</v>
-      </c>
-      <c r="F8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>63</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C9">
-        <v>1654</v>
-      </c>
-      <c r="D9" t="s">
-        <v>29</v>
-      </c>
       <c r="E9" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="F9" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="10" spans="1:6" ht="30">
+      <c r="A10" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="C10" s="14"/>
+      <c r="D10" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11">
+        <v>1654</v>
+      </c>
+      <c r="D11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
         <v>85</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B12" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C10">
+      <c r="C12">
         <v>1541</v>
       </c>
-      <c r="D10" t="s">
-        <v>29</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="D12" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" t="s">
         <v>44</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F12" t="s">
         <v>40</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated links and audience on some cards. Purple denotes a change. Added Stomach and Soft Tissue Sarcoma.
</commit_message>
<xml_diff>
--- a/Daisy-xls/IA/CTHP-Cards.xlsx
+++ b/Daisy-xls/IA/CTHP-Cards.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16040" tabRatio="655" firstSheet="16" activeTab="21"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16040" tabRatio="655" firstSheet="18" activeTab="23"/>
   </bookViews>
   <sheets>
     <sheet name="BRAIN" sheetId="6" r:id="rId1"/>
@@ -29,6 +29,8 @@
     <sheet name="SKIN" sheetId="20" r:id="rId20"/>
     <sheet name="MALIGNANT MESOTHELIOMA" sheetId="22" r:id="rId21"/>
     <sheet name="GALLBLADDER" sheetId="23" r:id="rId22"/>
+    <sheet name="STOMACH (GASTRIC)" sheetId="24" r:id="rId23"/>
+    <sheet name="SOFT TISSUE SARCOMA" sheetId="25" r:id="rId24"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -40,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2051" uniqueCount="506">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2252" uniqueCount="559">
   <si>
     <t>Title</t>
   </si>
@@ -1579,7 +1581,166 @@
     <t xml:space="preserve">Weight &amp; Activity </t>
   </si>
   <si>
-    <t>PAGE DOESN'T EXIST YET (/causes-prevention/risk-factors/weight-activity)</t>
+    <t>Gastric Cancer Treatment</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/pdq/treatment/gastric/Patient</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/pdq/treatment/gastric/HealthProfessional</t>
+  </si>
+  <si>
+    <t>Clinical Trials to Treat Stomach (Gastric) Cancer</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/clinicaltrials/search/results?protocolsearchid=9563172&amp;vers=1</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/druginfo/stomachcancer</t>
+  </si>
+  <si>
+    <t>Drugs Approved for Stomach (Gastric) Cancer</t>
+  </si>
+  <si>
+    <t>http://preview.cancer.gov/cancertopics/treatment/types/targeted-therapies</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/treatment/types/targeted-therapies/targeted-therapies-fact-sheet</t>
+  </si>
+  <si>
+    <t>Targeted Cancer Therapies</t>
+  </si>
+  <si>
+    <t>Stomach (Gastric) Cancer Prevention</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/pdq/prevention/gastric/Patient</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/pdq/prevention/gastric/HealthProfessional</t>
+  </si>
+  <si>
+    <t>PAGE DOES NOT EXIST YET: [cancer.gov/about-cancer/causes-prevention/risk-factors/infectious-agents]</t>
+  </si>
+  <si>
+    <t>http://preview.cancer.gov/cancertopics/causes-prevention/risk-factors/</t>
+  </si>
+  <si>
+    <t>PAGE DOESN'T EXIST YET [cancer.gov/cancertopics/causes-prevention/risk-factors/weight-activity)</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/causes-prevention/risk-factors/infectious-agents/h-pylori-fact-sheet</t>
+  </si>
+  <si>
+    <t>Helicobacter pylori and Cancer</t>
+  </si>
+  <si>
+    <t>Stomach (Gastric) Cancer Screening</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/pdq/screening/gastric/Patient</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/pdq/screening/gastric/HealthProfessional</t>
+  </si>
+  <si>
+    <t>Clinical Trials to Screen for Stomach (Gastric) Cancer</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/clinicaltrials/search/results?protocolsearchid=9234069&amp;vers=1</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/diagnosis-staging/understanding-lab-tests-fact-sheet</t>
+  </si>
+  <si>
+    <t>http://seer.cancer.gov/statfacts/html/stomach.html</t>
+  </si>
+  <si>
+    <t>Adult Soft Tissue Sarcoma Treatment</t>
+  </si>
+  <si>
+    <t>Childhood Soft Tissue Sarcoma Treatment</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/pdq/treatment/adult-soft-tissue-sarcoma/Patient</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/pdq/treatment/adult-soft-tissue-sarcoma/HealthProfessional</t>
+  </si>
+  <si>
+    <t>Gastrointestinal Stromal Tumors Treatment</t>
+  </si>
+  <si>
+    <t>Childhood Rhabdomyosarcoma Treatment</t>
+  </si>
+  <si>
+    <t>Kaposi Sarcoma Treatment</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/pdq/treatment/kaposis/Patient</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/pdq/treatment/kaposis/HealthProfessional</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/pdq/treatment/childrhabdomyosarcoma/Patient</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/pdq/treatment/childrhabdomyosarcoma/HealthProfessional</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/pdq/treatment/child-soft-tissue-sarcoma/HealthProfessional</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/pdq/treatment/child-soft-tissue-sarcoma/Patient</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/pdq/treatment/gist/Patient</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/pdq/treatment/gist/HealthProfessional</t>
+  </si>
+  <si>
+    <t>Clinical Trials to Treat Adult Soft Tissue Sarcoma</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/clinicaltrials/search/results?protocolsearchid=10223845&amp;vers=1</t>
+  </si>
+  <si>
+    <t>Drugs Approved for Soft Tissue Sarcoma</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/druginfo/softtissuesarcoma</t>
+  </si>
+  <si>
+    <t>Drugs Approved for Gastrointestinal Stromal Tumors</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/druginfo/GIST</t>
+  </si>
+  <si>
+    <t>Drugs Approved for Rhabdomyosarcoma</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/druginfo/rhabdomyosarcoma</t>
+  </si>
+  <si>
+    <t>Drugs Approved for Kaposi Sarcoma</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/druginfo/kaposi-sarcoma</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/causes-prevention/risk-factors/infectious-agents/hiv-fact-sheet</t>
+  </si>
+  <si>
+    <t>HIV Infection and Cancer Risk</t>
+  </si>
+  <si>
+    <t>Clinical Trials to Treat Kaposi Sarcoma</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/clinicaltrials/search/results?protocolsearchid=8001163&amp;vers=1</t>
   </si>
 </sst>
 </file>
@@ -1647,7 +1808,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1690,6 +1851,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD3A5FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD3A5FF"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -1715,7 +1888,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="323">
+  <cellStyleXfs count="375">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2039,8 +2212,60 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2100,8 +2325,10 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="323">
+  <cellStyles count="375">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2312,6 +2539,32 @@
     <cellStyle name="Followed Hyperlink" xfId="320" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="321" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="322" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="324" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="326" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="328" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="330" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="332" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="334" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="336" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="338" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="340" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="342" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="344" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="346" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="348" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="350" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="352" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="354" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="356" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="358" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="360" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="362" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="364" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="366" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="368" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="370" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="372" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="374" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2424,6 +2677,32 @@
     <cellStyle name="Hyperlink" xfId="264" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="266" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="268" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="323" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="325" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="327" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="329" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="331" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="333" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="335" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="337" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="339" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="341" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="343" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="345" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="347" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="349" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="351" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="353" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="355" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="357" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="359" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="361" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="363" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="365" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="367" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="369" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="371" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="373" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2760,10 +3039,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection sqref="A1:XFD1"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1:C1048576"/>
+      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2776,7 +3055,7 @@
     <col min="6" max="6" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="17.25">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="32">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -3032,8 +3311,8 @@
       <c r="E13" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="F13" s="15" t="s">
-        <v>41</v>
+      <c r="F13" s="33" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -3292,8 +3571,8 @@
       <c r="E26" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="F26" s="15" t="s">
-        <v>41</v>
+      <c r="F26" s="33" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -3588,8 +3867,8 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1:C1048576"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3600,7 +3879,7 @@
     <col min="6" max="6" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="17.25">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="16">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3680,7 +3959,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="31.5">
+    <row r="5" spans="1:6" ht="30">
       <c r="A5" s="2" t="s">
         <v>102</v>
       </c>
@@ -3780,7 +4059,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="31.5">
+    <row r="10" spans="1:6" ht="30">
       <c r="A10" s="2" t="s">
         <v>119</v>
       </c>
@@ -3798,7 +4077,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="31.5">
+    <row r="11" spans="1:6" ht="30">
       <c r="A11" s="2" t="s">
         <v>120</v>
       </c>
@@ -3816,7 +4095,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="31.5">
+    <row r="12" spans="1:6" ht="30">
       <c r="A12" s="2" t="s">
         <v>122</v>
       </c>
@@ -3834,7 +4113,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="31.5">
+    <row r="13" spans="1:6" ht="30">
       <c r="A13" s="2" t="s">
         <v>124</v>
       </c>
@@ -3852,7 +4131,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="31.5">
+    <row r="14" spans="1:6" ht="30">
       <c r="A14" s="2" t="s">
         <v>130</v>
       </c>
@@ -3870,7 +4149,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="31.5">
+    <row r="15" spans="1:6" ht="30">
       <c r="A15" s="2" t="s">
         <v>128</v>
       </c>
@@ -3888,7 +4167,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="31.5">
+    <row r="16" spans="1:6" ht="30">
       <c r="A16" s="2" t="s">
         <v>126</v>
       </c>
@@ -3906,7 +4185,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="31.5">
+    <row r="17" spans="1:6" ht="30">
       <c r="A17" s="2" t="s">
         <v>132</v>
       </c>
@@ -3920,11 +4199,11 @@
       <c r="E17" t="s">
         <v>37</v>
       </c>
-      <c r="F17" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="31.5">
+      <c r="F17" s="33" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="30">
       <c r="A18" s="2" t="s">
         <v>134</v>
       </c>
@@ -3938,11 +4217,11 @@
       <c r="E18" t="s">
         <v>37</v>
       </c>
-      <c r="F18" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="31.5">
+      <c r="F18" s="33" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="30">
       <c r="A19" s="2" t="s">
         <v>135</v>
       </c>
@@ -3956,8 +4235,8 @@
       <c r="E19" t="s">
         <v>37</v>
       </c>
-      <c r="F19" t="s">
-        <v>41</v>
+      <c r="F19" s="33" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -3996,8 +4275,8 @@
       <c r="E21" t="s">
         <v>43</v>
       </c>
-      <c r="F21" t="s">
-        <v>41</v>
+      <c r="F21" s="33" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -4093,7 +4372,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="31.5">
+    <row r="27" spans="1:6" ht="30">
       <c r="A27" s="2" t="s">
         <v>102</v>
       </c>
@@ -4153,7 +4432,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="31.5">
+    <row r="30" spans="1:6" ht="30">
       <c r="A30" s="2" t="s">
         <v>111</v>
       </c>
@@ -4193,7 +4472,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="31.5">
+    <row r="32" spans="1:6">
       <c r="A32" t="s">
         <v>63</v>
       </c>
@@ -4250,7 +4529,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1:C1048576"/>
+      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4262,7 +4541,7 @@
     <col min="6" max="6" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="17.25">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="16">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4302,7 +4581,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="31.5">
+    <row r="3" spans="1:6" ht="30">
       <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
@@ -4322,7 +4601,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="31.5">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>307</v>
       </c>
@@ -4376,8 +4655,8 @@
       <c r="E6" t="s">
         <v>43</v>
       </c>
-      <c r="F6" t="s">
-        <v>41</v>
+      <c r="F6" s="33" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -4400,7 +4679,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="31.5">
+    <row r="8" spans="1:6" ht="30">
       <c r="A8" s="5" t="s">
         <v>304</v>
       </c>
@@ -4420,7 +4699,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="31.5">
+    <row r="9" spans="1:6" ht="30">
       <c r="A9" s="5" t="s">
         <v>2</v>
       </c>
@@ -4496,7 +4775,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4508,7 +4787,7 @@
     <col min="6" max="6" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="17.25">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="16">
       <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
@@ -4548,7 +4827,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="31.5">
+    <row r="3" spans="1:6" ht="30">
       <c r="A3" s="14" t="s">
         <v>2</v>
       </c>
@@ -4568,7 +4847,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="31.5">
+    <row r="4" spans="1:6" ht="30">
       <c r="A4" s="15" t="s">
         <v>313</v>
       </c>
@@ -4646,7 +4925,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="31.5">
+    <row r="8" spans="1:6" ht="30">
       <c r="A8" s="15" t="s">
         <v>320</v>
       </c>
@@ -4680,8 +4959,8 @@
       <c r="E9" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="F9" s="15" t="s">
-        <v>41</v>
+      <c r="F9" s="33" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -4698,8 +4977,8 @@
       <c r="E10" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="F10" s="15" t="s">
-        <v>41</v>
+      <c r="F10" s="33" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="5" customFormat="1">
@@ -4742,7 +5021,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="5" customFormat="1" ht="31.5">
+    <row r="13" spans="1:6" s="5" customFormat="1" ht="30">
       <c r="A13" s="14" t="s">
         <v>329</v>
       </c>
@@ -4762,7 +5041,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="31.5">
+    <row r="14" spans="1:6" ht="30">
       <c r="A14" s="14" t="s">
         <v>330</v>
       </c>
@@ -4780,7 +5059,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="31.5">
+    <row r="15" spans="1:6" ht="30">
       <c r="A15" s="14" t="s">
         <v>331</v>
       </c>
@@ -4812,8 +5091,8 @@
       <c r="E16" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="F16" s="14" t="s">
-        <v>41</v>
+      <c r="F16" s="33" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -4830,7 +5109,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:6" s="5" customFormat="1" ht="31.5">
+    <row r="18" spans="1:6" s="5" customFormat="1" ht="30">
       <c r="A18" s="14" t="s">
         <v>310</v>
       </c>
@@ -4850,7 +5129,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:6" s="5" customFormat="1" ht="31.5">
+    <row r="19" spans="1:6" s="5" customFormat="1" ht="30">
       <c r="A19" s="14" t="s">
         <v>2</v>
       </c>
@@ -4870,7 +5149,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:6" s="5" customFormat="1" ht="31.5">
+    <row r="20" spans="1:6" s="5" customFormat="1" ht="30">
       <c r="A20" s="14" t="s">
         <v>317</v>
       </c>
@@ -4890,7 +5169,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:6" s="5" customFormat="1" ht="31.5">
+    <row r="21" spans="1:6" s="5" customFormat="1" ht="30">
       <c r="A21" s="14" t="s">
         <v>323</v>
       </c>
@@ -4927,7 +5206,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A16" sqref="A16:F17"/>
+      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4939,7 +5218,7 @@
     <col min="6" max="6" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="17.25">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="16">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4979,7 +5258,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="31.5">
+    <row r="3" spans="1:6" ht="30">
       <c r="A3" s="16" t="s">
         <v>356</v>
       </c>
@@ -5035,7 +5314,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="5" customFormat="1" ht="31.5">
+    <row r="6" spans="1:6" s="5" customFormat="1" ht="30">
       <c r="A6" s="18" t="s">
         <v>365</v>
       </c>
@@ -5055,7 +5334,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="31.5">
+    <row r="7" spans="1:6" ht="30">
       <c r="A7" s="16" t="s">
         <v>364</v>
       </c>
@@ -5149,8 +5428,8 @@
       <c r="E11" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="F11" s="15" t="s">
-        <v>41</v>
+      <c r="F11" s="33" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -5213,7 +5492,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:6" s="5" customFormat="1" ht="31.5">
+    <row r="15" spans="1:6" s="5" customFormat="1" ht="30">
       <c r="A15" s="18" t="s">
         <v>365</v>
       </c>
@@ -5290,7 +5569,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
+      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5302,7 +5581,7 @@
     <col min="6" max="6" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="17.25">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="16">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5362,7 +5641,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="5" customFormat="1" ht="31.5">
+    <row r="4" spans="1:6" s="5" customFormat="1" ht="30">
       <c r="A4" s="14" t="s">
         <v>2</v>
       </c>
@@ -5382,7 +5661,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="31.5">
+    <row r="5" spans="1:6" ht="30">
       <c r="A5" s="15" t="s">
         <v>377</v>
       </c>
@@ -5400,7 +5679,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="31.5">
+    <row r="6" spans="1:6" ht="30">
       <c r="A6" s="15" t="s">
         <v>378</v>
       </c>
@@ -5478,7 +5757,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="31.5">
+    <row r="10" spans="1:6" ht="30">
       <c r="A10" s="15" t="s">
         <v>386</v>
       </c>
@@ -5496,7 +5775,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="31.5">
+    <row r="11" spans="1:6" ht="30">
       <c r="A11" s="15" t="s">
         <v>387</v>
       </c>
@@ -5537,7 +5816,7 @@
         <v>64</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>69</v>
+        <v>519</v>
       </c>
       <c r="C13" s="15">
         <v>899999</v>
@@ -5548,8 +5827,8 @@
       <c r="E13" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="F13" s="15" t="s">
-        <v>41</v>
+      <c r="F13" s="33" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:6" s="5" customFormat="1">
@@ -5572,7 +5851,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="31.5">
+    <row r="15" spans="1:6" ht="30">
       <c r="A15" s="14" t="s">
         <v>401</v>
       </c>
@@ -5624,8 +5903,8 @@
       <c r="E17" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="F17" s="14" t="s">
-        <v>41</v>
+      <c r="F17" s="33" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -5682,7 +5961,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:6" s="5" customFormat="1" ht="31.5">
+    <row r="21" spans="1:6" s="5" customFormat="1" ht="30">
       <c r="A21" s="14" t="s">
         <v>2</v>
       </c>
@@ -5702,7 +5981,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:6" s="5" customFormat="1" ht="31.5">
+    <row r="22" spans="1:6" s="5" customFormat="1">
       <c r="A22" s="14" t="s">
         <v>382</v>
       </c>
@@ -5815,9 +6094,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1"/>
+      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5830,7 +6109,7 @@
     <col min="6" max="6" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="17.25">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="32">
       <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
@@ -5870,7 +6149,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="5" customFormat="1" ht="31.5">
+    <row r="3" spans="1:6" s="5" customFormat="1">
       <c r="A3" s="18" t="s">
         <v>2</v>
       </c>
@@ -5924,8 +6203,8 @@
       <c r="E5" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="F5" s="15" t="s">
-        <v>41</v>
+      <c r="F5" s="33" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="5" customFormat="1">
@@ -6000,11 +6279,11 @@
       <c r="E9" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="F9" s="12" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" s="5" customFormat="1" ht="31.5">
+      <c r="F9" s="33" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" s="5" customFormat="1" ht="30">
       <c r="A10" s="12" t="s">
         <v>10</v>
       </c>
@@ -6018,11 +6297,11 @@
       <c r="E10" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="F10" s="12" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" s="5" customFormat="1" ht="31.5">
+      <c r="F10" s="33" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" s="5" customFormat="1" ht="30">
       <c r="A11" s="18" t="s">
         <v>420</v>
       </c>
@@ -6036,8 +6315,8 @@
       <c r="E11" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="F11" s="12" t="s">
-        <v>41</v>
+      <c r="F11" s="33" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:6" s="5" customFormat="1">
@@ -6112,7 +6391,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:6" s="5" customFormat="1" ht="31.5">
+    <row r="16" spans="1:6" s="5" customFormat="1" ht="30">
       <c r="A16" s="18" t="s">
         <v>2</v>
       </c>
@@ -6189,7 +6468,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8:F9"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6284,7 +6563,7 @@
         <v>64</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>69</v>
+        <v>519</v>
       </c>
       <c r="C5" s="15">
         <v>899999</v>
@@ -6295,8 +6574,8 @@
       <c r="E5" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="F5" s="15" t="s">
-        <v>41</v>
+      <c r="F5" s="33" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -6394,7 +6673,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A9" sqref="A9:F10"/>
+      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6454,7 +6733,9 @@
       <c r="C3" s="11"/>
       <c r="D3" s="15"/>
       <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
+      <c r="F3" s="15" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="15" t="s">
@@ -6501,7 +6782,7 @@
         <v>64</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>69</v>
+        <v>519</v>
       </c>
       <c r="C6" s="15">
         <v>899999</v>
@@ -6512,8 +6793,8 @@
       <c r="E6" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="F6" s="15" t="s">
-        <v>41</v>
+      <c r="F6" s="34" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -6611,7 +6892,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A10" sqref="A10:F11"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6746,7 +7027,7 @@
         <v>64</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>69</v>
+        <v>519</v>
       </c>
       <c r="C7" s="15">
         <v>899999</v>
@@ -6757,8 +7038,8 @@
       <c r="E7" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="F7" s="15" t="s">
-        <v>41</v>
+      <c r="F7" s="34" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -6856,7 +7137,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A9" sqref="A9:F10"/>
+      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6969,7 +7250,7 @@
         <v>64</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>69</v>
+        <v>519</v>
       </c>
       <c r="C6" s="15">
         <v>899999</v>
@@ -6980,8 +7261,8 @@
       <c r="E6" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="F6" s="15" t="s">
-        <v>41</v>
+      <c r="F6" s="34" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -7080,7 +7361,7 @@
     <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection sqref="A1:XFD1"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1:C1048576"/>
+      <selection pane="bottomLeft" activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -7093,7 +7374,7 @@
     <col min="6" max="6" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="17.25">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="32">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -7173,7 +7454,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="31.5">
+    <row r="5" spans="1:6">
       <c r="A5" s="15" t="s">
         <v>203</v>
       </c>
@@ -7251,7 +7532,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" ht="30">
       <c r="A9" s="16" t="s">
         <v>209</v>
       </c>
@@ -7307,8 +7588,8 @@
       <c r="E11" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="F11" s="15" t="s">
-        <v>41</v>
+      <c r="F11" s="33" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -7351,7 +7632,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="31.5">
+    <row r="14" spans="1:6" ht="30">
       <c r="A14" s="14" t="s">
         <v>213</v>
       </c>
@@ -7405,7 +7686,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="31.5">
+    <row r="17" spans="1:6" ht="30">
       <c r="A17" s="15" t="s">
         <v>199</v>
       </c>
@@ -7445,7 +7726,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="31.5">
+    <row r="19" spans="1:6" ht="30">
       <c r="A19" s="15" t="s">
         <v>209</v>
       </c>
@@ -7485,7 +7766,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="31.5">
+    <row r="21" spans="1:6">
       <c r="A21" s="14" t="s">
         <v>211</v>
       </c>
@@ -7541,7 +7822,7 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -7809,8 +8090,8 @@
       <c r="E14" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="F14" s="15" t="s">
-        <v>41</v>
+      <c r="F14" s="34" t="s">
+        <v>39</v>
       </c>
       <c r="G14" s="32" t="s">
         <v>477</v>
@@ -7884,8 +8165,8 @@
       <c r="E18" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="F18" s="15" t="s">
-        <v>41</v>
+      <c r="F18" s="34" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -8045,7 +8326,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1"/>
+      <selection pane="bottomLeft" activeCell="A10" sqref="A10:F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -8205,8 +8486,8 @@
       <c r="E8" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="F8" s="15" t="s">
-        <v>41</v>
+      <c r="F8" s="34" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -8214,7 +8495,7 @@
         <v>64</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>69</v>
+        <v>519</v>
       </c>
       <c r="C9" s="15">
         <v>899999</v>
@@ -8225,8 +8506,8 @@
       <c r="E9" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="F9" s="15" t="s">
-        <v>41</v>
+      <c r="F9" s="34" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -8342,15 +8623,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B20" sqref="B20"/>
+      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="39" customWidth="1"/>
-    <col min="2" max="2" width="76.5" customWidth="1"/>
+    <col min="2" max="2" width="91.1640625" customWidth="1"/>
     <col min="4" max="4" width="25" customWidth="1"/>
     <col min="5" max="5" width="20" customWidth="1"/>
     <col min="6" max="6" width="14.83203125" customWidth="1"/>
@@ -8457,7 +8738,7 @@
         <v>504</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>505</v>
+        <v>520</v>
       </c>
       <c r="C6" s="28"/>
       <c r="D6" s="15" t="s">
@@ -8466,8 +8747,8 @@
       <c r="E6" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="F6" s="15" t="s">
-        <v>41</v>
+      <c r="F6" s="34" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -8475,7 +8756,7 @@
         <v>64</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>69</v>
+        <v>519</v>
       </c>
       <c r="C7" s="15">
         <v>899999</v>
@@ -8486,8 +8767,8 @@
       <c r="E7" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="F7" s="15" t="s">
-        <v>41</v>
+      <c r="F7" s="34" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -8565,6 +8846,792 @@
         <v>44</v>
       </c>
       <c r="F11" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A13" sqref="A13:F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="50.83203125" customWidth="1"/>
+    <col min="2" max="2" width="88.1640625" customWidth="1"/>
+    <col min="4" max="4" width="25.6640625" customWidth="1"/>
+    <col min="5" max="5" width="22.33203125" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="16">
+      <c r="A1" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="15" t="s">
+        <v>505</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>506</v>
+      </c>
+      <c r="C2" s="28"/>
+      <c r="D2" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="15" t="s">
+        <v>508</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>509</v>
+      </c>
+      <c r="C3" s="11"/>
+      <c r="D3" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="15" t="s">
+        <v>511</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>510</v>
+      </c>
+      <c r="C4" s="28"/>
+      <c r="D4" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>512</v>
+      </c>
+      <c r="C5" s="28"/>
+      <c r="D5" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="15" t="s">
+        <v>515</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>516</v>
+      </c>
+      <c r="C6" s="28"/>
+      <c r="D6" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="15" t="s">
+        <v>321</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>518</v>
+      </c>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="15" t="s">
+        <v>523</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>524</v>
+      </c>
+      <c r="C8" s="28"/>
+      <c r="D8" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="15" t="s">
+        <v>526</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>527</v>
+      </c>
+      <c r="C9" s="28"/>
+      <c r="D9" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="15" t="s">
+        <v>213</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>528</v>
+      </c>
+      <c r="C10" s="11"/>
+      <c r="D10" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="15"/>
+      <c r="B11" s="15" t="s">
+        <v>529</v>
+      </c>
+      <c r="C11" s="11"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="15" t="s">
+        <v>505</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>507</v>
+      </c>
+      <c r="C12" s="28"/>
+      <c r="D12" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="15" t="s">
+        <v>514</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>513</v>
+      </c>
+      <c r="C13" s="28"/>
+      <c r="D13" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="15" t="s">
+        <v>515</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>517</v>
+      </c>
+      <c r="C14" s="28"/>
+      <c r="D14" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="15" t="s">
+        <v>522</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>521</v>
+      </c>
+      <c r="C15" s="28"/>
+      <c r="D15" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F15" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="15" t="s">
+        <v>523</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>525</v>
+      </c>
+      <c r="C16" s="28"/>
+      <c r="D16" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="F16" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B27" sqref="B27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="42.1640625" customWidth="1"/>
+    <col min="2" max="2" width="86.6640625" customWidth="1"/>
+    <col min="4" max="4" width="28.6640625" customWidth="1"/>
+    <col min="5" max="5" width="23.33203125" customWidth="1"/>
+    <col min="6" max="6" width="15.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="16">
+      <c r="A1" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="15" t="s">
+        <v>530</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>532</v>
+      </c>
+      <c r="C2" s="28"/>
+      <c r="D2" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="15" t="s">
+        <v>531</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>542</v>
+      </c>
+      <c r="C3" s="28"/>
+      <c r="D3" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="15" t="s">
+        <v>534</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>543</v>
+      </c>
+      <c r="C4" s="28"/>
+      <c r="D4" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="15" t="s">
+        <v>535</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>539</v>
+      </c>
+      <c r="C5" s="28"/>
+      <c r="D5" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="15" t="s">
+        <v>536</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>537</v>
+      </c>
+      <c r="C6" s="28"/>
+      <c r="D6" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="15" t="s">
+        <v>545</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>546</v>
+      </c>
+      <c r="C7" s="11"/>
+      <c r="D7" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="15" t="s">
+        <v>557</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>558</v>
+      </c>
+      <c r="C8" s="11"/>
+      <c r="D8" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="15" t="s">
+        <v>547</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>548</v>
+      </c>
+      <c r="C9" s="28"/>
+      <c r="D9" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="15" t="s">
+        <v>549</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>550</v>
+      </c>
+      <c r="C10" s="28"/>
+      <c r="D10" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="15" t="s">
+        <v>551</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>552</v>
+      </c>
+      <c r="C11" s="28"/>
+      <c r="D11" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="15" t="s">
+        <v>553</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>554</v>
+      </c>
+      <c r="C12" s="28"/>
+      <c r="D12" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>512</v>
+      </c>
+      <c r="C13" s="28"/>
+      <c r="D13" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="C14" s="15">
+        <v>6158</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="15" t="s">
+        <v>556</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>555</v>
+      </c>
+      <c r="C15" s="28"/>
+      <c r="D15" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F15" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="C16" s="15">
+        <v>6145</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="F16" s="15" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="15" t="s">
+        <v>530</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>533</v>
+      </c>
+      <c r="C17" s="28"/>
+      <c r="D17" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F17" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="15" t="s">
+        <v>531</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>541</v>
+      </c>
+      <c r="C18" s="28"/>
+      <c r="D18" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F18" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="15" t="s">
+        <v>534</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>544</v>
+      </c>
+      <c r="C19" s="28"/>
+      <c r="D19" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F19" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="15" t="s">
+        <v>535</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>540</v>
+      </c>
+      <c r="C20" s="28"/>
+      <c r="D20" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F20" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="15" t="s">
+        <v>536</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>538</v>
+      </c>
+      <c r="C21" s="28"/>
+      <c r="D21" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F21" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="15" t="s">
+        <v>514</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>513</v>
+      </c>
+      <c r="C22" s="28"/>
+      <c r="D22" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F22" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="B23" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="C23" s="15">
+        <v>1654</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E23" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F23" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24" s="15">
+        <v>1541</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E24" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="F24" s="15" t="s">
         <v>40</v>
       </c>
     </row>
@@ -8586,7 +9653,7 @@
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection sqref="A1:XFD1"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1:C1048576"/>
+      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -8599,7 +9666,7 @@
     <col min="6" max="6" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="17.25">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="32">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -8753,8 +9820,8 @@
       <c r="E8" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="F8" s="15" t="s">
-        <v>41</v>
+      <c r="F8" s="33" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -8909,7 +9976,7 @@
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection sqref="A1:XFD1"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1:C1048576"/>
+      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -8922,7 +9989,7 @@
     <col min="6" max="7" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" ht="17.25">
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="32">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -9081,8 +10148,8 @@
       <c r="E8" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="F8" s="15" t="s">
-        <v>41</v>
+      <c r="F8" s="33" t="s">
+        <v>39</v>
       </c>
       <c r="G8" s="15"/>
     </row>
@@ -9247,7 +10314,7 @@
     <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection sqref="A1:XFD1"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1:C1048576"/>
+      <selection pane="bottomLeft" activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -9260,7 +10327,7 @@
     <col min="6" max="6" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="17.25">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="32">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -9414,8 +10481,8 @@
       <c r="E8" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="F8" s="15" t="s">
-        <v>41</v>
+      <c r="F8" s="33" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -9610,8 +10677,8 @@
       <c r="E18" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="F18" s="15" t="s">
-        <v>41</v>
+      <c r="F18" s="33" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -9708,8 +10775,8 @@
       <c r="E23" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="F23" s="15" t="s">
-        <v>41</v>
+      <c r="F23" s="33" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -9744,8 +10811,8 @@
       <c r="E25" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="F25" s="20" t="s">
-        <v>41</v>
+      <c r="F25" s="33" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -9967,7 +11034,7 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1:C1048576"/>
+      <selection pane="bottomLeft" activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -9982,7 +11049,7 @@
     <col min="8" max="16384" width="11" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="17.25">
+    <row r="1" spans="1:7" ht="16">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -10019,8 +11086,8 @@
       <c r="E2" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="F2" s="12" t="s">
-        <v>41</v>
+      <c r="F2" s="33" t="s">
+        <v>39</v>
       </c>
       <c r="G2" s="12"/>
     </row>
@@ -10353,8 +11420,8 @@
       <c r="E18" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="F18" s="20" t="s">
-        <v>41</v>
+      <c r="F18" s="33" t="s">
+        <v>39</v>
       </c>
       <c r="G18" s="8"/>
     </row>
@@ -10416,8 +11483,8 @@
       <c r="E21" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="F21" s="12" t="s">
-        <v>41</v>
+      <c r="F21" s="33" t="s">
+        <v>39</v>
       </c>
       <c r="G21" s="12"/>
     </row>
@@ -10435,8 +11502,8 @@
       <c r="E22" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="F22" s="12" t="s">
-        <v>41</v>
+      <c r="F22" s="33" t="s">
+        <v>39</v>
       </c>
       <c r="G22" s="12"/>
     </row>
@@ -10456,8 +11523,8 @@
       <c r="E23" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="F23" s="8" t="s">
-        <v>41</v>
+      <c r="F23" s="33" t="s">
+        <v>39</v>
       </c>
       <c r="G23" s="8"/>
     </row>
@@ -10542,7 +11609,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1:C1048576"/>
+      <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -10555,7 +11622,7 @@
     <col min="6" max="6" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="17.25">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="32">
       <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
@@ -10595,7 +11662,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="31.5">
+    <row r="3" spans="1:6" ht="30">
       <c r="A3" s="15" t="s">
         <v>2</v>
       </c>
@@ -10689,8 +11756,8 @@
       <c r="E7" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="F7" s="15" t="s">
-        <v>41</v>
+      <c r="F7" s="33" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -10733,7 +11800,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="31.5">
+    <row r="10" spans="1:6" ht="30">
       <c r="A10" s="15" t="s">
         <v>2</v>
       </c>
@@ -10810,7 +11877,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1:C1048576"/>
+      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -10822,7 +11889,7 @@
     <col min="6" max="6" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="17.25">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="16">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -10862,7 +11929,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="31.5">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>76</v>
       </c>
@@ -10956,8 +12023,8 @@
       <c r="E7" t="s">
         <v>43</v>
       </c>
-      <c r="F7" t="s">
-        <v>41</v>
+      <c r="F7" s="33" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -11069,7 +12136,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1:C1048576"/>
+      <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -11080,7 +12147,7 @@
     <col min="5" max="6" width="23.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="17.25">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="16">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -11214,8 +12281,8 @@
       <c r="E7" t="s">
         <v>43</v>
       </c>
-      <c r="F7" t="s">
-        <v>41</v>
+      <c r="F7" s="33" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -11258,7 +12325,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="31.5">
+    <row r="10" spans="1:6" ht="30">
       <c r="A10" s="5" t="s">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
All but Head & Neck and Lymphoma.
</commit_message>
<xml_diff>
--- a/Daisy-xls/IA/CTHP-Cards.xlsx
+++ b/Daisy-xls/IA/CTHP-Cards.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16040" tabRatio="655" firstSheet="25" activeTab="31"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16040" tabRatio="655" firstSheet="36" activeTab="43"/>
   </bookViews>
   <sheets>
     <sheet name="BRAIN" sheetId="6" r:id="rId1"/>
@@ -39,6 +39,18 @@
     <sheet name="OVARIAN" sheetId="31" r:id="rId30"/>
     <sheet name="PHEOCHROMOCYTOMA" sheetId="32" r:id="rId31"/>
     <sheet name="PARATHYROID" sheetId="33" r:id="rId32"/>
+    <sheet name="PENILE" sheetId="34" r:id="rId33"/>
+    <sheet name="PITUITARY TUMOR" sheetId="35" r:id="rId34"/>
+    <sheet name="PROSTATE" sheetId="36" r:id="rId35"/>
+    <sheet name="SMALL INTESTINE" sheetId="37" r:id="rId36"/>
+    <sheet name="TESTICULAR" sheetId="38" r:id="rId37"/>
+    <sheet name="THYMOMA &amp; THYMIC CARCINOMA" sheetId="39" r:id="rId38"/>
+    <sheet name="THYROID" sheetId="40" r:id="rId39"/>
+    <sheet name="URETHRAL" sheetId="41" r:id="rId40"/>
+    <sheet name="UTERINE" sheetId="42" r:id="rId41"/>
+    <sheet name="VAGINAL" sheetId="43" r:id="rId42"/>
+    <sheet name="VULVAR" sheetId="44" r:id="rId43"/>
+    <sheet name="LANGERHANS CELL HISTIOCYTOSIS" sheetId="45" r:id="rId44"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -50,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3018" uniqueCount="670">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3913" uniqueCount="796">
   <si>
     <t>Title</t>
   </si>
@@ -2082,6 +2094,384 @@
   </si>
   <si>
     <t>Radiation Therapy for Cancer</t>
+  </si>
+  <si>
+    <t>Penile Cancer Treatment</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/pdq/treatment/penile/Patient</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/pdq/treatment/penile/HealthProfessional</t>
+  </si>
+  <si>
+    <t>Clinical Trials to Treat Penile Cancer</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/clinicaltrials/search/results?protocolsearchid=10403383&amp;vers=1</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/druginfo/penilecancer</t>
+  </si>
+  <si>
+    <t>Drugs Approved for Penile Cancer</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/treatment/types/surgery/lasers-fact-sheet</t>
+  </si>
+  <si>
+    <t>Lasers in Cancer Treatment</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/pdq/treatment/pituitary/Patient</t>
+  </si>
+  <si>
+    <t>Pituitary Tumors Treatment</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/pdq/treatment/pituitary/HealthProfessional</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/clinicaltrials/search/results?protocolsearchid=6193467&amp;vers=1</t>
+  </si>
+  <si>
+    <t>Clinical Trials to Treat Pituitary Tumors</t>
+  </si>
+  <si>
+    <t>Prostate Cancer Treatment</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/pdq/treatment/prostate/Patient</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/pdq/treatment/prostate/HealthProfessional</t>
+  </si>
+  <si>
+    <t>Clinical Trials to Treat Prostate Cancer</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/clinicaltrials/search/results?protocolsearchid=6199488&amp;vers=1</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/druginfo/prostatecancer</t>
+  </si>
+  <si>
+    <t>Drugs Approved for Prostate Cancer</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/types/prostate/prostate-hormone-therapy-fact-sheet</t>
+  </si>
+  <si>
+    <t>Hormone Therapy for Prostate Cancer</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/publications/patient-education/understanding-prostate-cancer-treatment</t>
+  </si>
+  <si>
+    <t>Treatment Choices for Men With Early-Stage Prostate Cancer</t>
+  </si>
+  <si>
+    <t>Cancer Vaccines</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/causes-prevention/vaccines-fact-sheet</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/treatment/types/surgery/cryosurgery-fact-sheet</t>
+  </si>
+  <si>
+    <t>Prostate Cancer Prevention</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/pdq/prevention/prostate/Patient</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/pdq/prevention/prostate/healthprofessional</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/pdq/cam/prostatesupplements/Patient</t>
+  </si>
+  <si>
+    <t>Prostate Cancer, Nutrition, and Dietary Supplements</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/pdq/cam/prostatesupplements/healthprofessional</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/clinicaltrials/search/results?protocolsearchid=6138004&amp;vers=1</t>
+  </si>
+  <si>
+    <t>Clinical Trials to Prevent Prostate Cancer</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/pdq/genetics/prostate/HealthProfessional</t>
+  </si>
+  <si>
+    <t>Genetics of Prostate Cancer</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/pdq/screening/prostate/Patient</t>
+  </si>
+  <si>
+    <t>Prostate Cancer Screening</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/pdq/screening/prostate/HealthProfessional</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/types/prostate/psa-fact-sheet</t>
+  </si>
+  <si>
+    <t>Prostate-Specific Antigen (PSA) Test</t>
+  </si>
+  <si>
+    <t>Clinical Trials to Screen for Prostate Cancer</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/clinicaltrials/search/results?protocolsearchid=6175284&amp;vers=1</t>
+  </si>
+  <si>
+    <t>Understanding Prostate Changes</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/screening/understanding-prostate-changes/</t>
+  </si>
+  <si>
+    <t>http://seer.cancer.gov/statfacts/html/prost.html</t>
+  </si>
+  <si>
+    <t>Small Intestine Cancer Treatment</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/pdq/treatment/smallintestine/Patient</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/pdq/treatment/smallintestine/HealthProfessional</t>
+  </si>
+  <si>
+    <t>http://seer.cancer.gov/statfacts/html/smint.html</t>
+  </si>
+  <si>
+    <t>Testicular Cancer Treatment</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/pdq/treatment/testicular/Patient</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/pdq/treatment/testicular/HealthProfessional</t>
+  </si>
+  <si>
+    <t>Clinical Trials to Treat Testicular Cancer</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/clinicaltrials/search/results?protocolsearchid=13848549&amp;vers=1</t>
+  </si>
+  <si>
+    <t>Drugs Approved for Testicular Cancer</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/druginfo/testicularcancer</t>
+  </si>
+  <si>
+    <t>http://familial-testicular-cancer.cancer.gov/index.html</t>
+  </si>
+  <si>
+    <t>Familial Testicular Cancer</t>
+  </si>
+  <si>
+    <t>Testicular Cancer Screening</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/pdq/screening/testicular/Patient</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/pdq/screening/testicular/HealthProfessional</t>
+  </si>
+  <si>
+    <t>Understanding Laboratory Results</t>
+  </si>
+  <si>
+    <t>http://seer.cancer.gov/statfacts/html/testis.html</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/pdq/treatment/thymoma/patient</t>
+  </si>
+  <si>
+    <t>Thymoma and Thymic Carcinoma Treatment</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/pdq/treatment/thymoma/HealthProfessional</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/clinicaltrials/search/results?protocolsearchid=10403490&amp;vers=1</t>
+  </si>
+  <si>
+    <t>Clinical Trials to Treat Thymoma and Thymic Carcinoma</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/pdq/treatment/thyroid/Patient</t>
+  </si>
+  <si>
+    <t>Thyroid Cancer Treatment</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/pdq/treatment/thyroid/HealthProfessional</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/clinicaltrials/search/results?protocolsearchid=6200083&amp;vers=1</t>
+  </si>
+  <si>
+    <t>Clinical Trials to Treat Thyroid Cancer</t>
+  </si>
+  <si>
+    <t>Drugs Approved for Thyroid Cancer</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/druginfo/thyroidcancer</t>
+  </si>
+  <si>
+    <t>Radiation Therapy</t>
+  </si>
+  <si>
+    <t>DOESN'T EXIST YET [cancer.gov/cancertopics/treatment/types/radiation]</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/pdq/genetics/medullarythyroid/HealthProfessional</t>
+  </si>
+  <si>
+    <t>Genetics of Endocrine and Neuroendocrine Neoplasias</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/causes-prevention/risk-factors/radiation/i-131</t>
+  </si>
+  <si>
+    <t>Get the Facts About Exposure to I-131 Radiation</t>
+  </si>
+  <si>
+    <t>http://seer.cancer.gov/statfacts/html/thyro.html</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/pdq/treatment/urethral/Patient</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/pdq/treatment/urethral/HealthProfessional</t>
+  </si>
+  <si>
+    <t>Urethral Cancer Treatment</t>
+  </si>
+  <si>
+    <t>Uterine Sarcoma Treatment</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/pdq/treatment/uterinesarcoma/Patient</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/pdq/treatment/uterinesarcoma/HealthProfessional</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/pdq/treatment/endometrial/HealthProfessional</t>
+  </si>
+  <si>
+    <t>Endometrial Cancer Treatemtn</t>
+  </si>
+  <si>
+    <t>Endometrial Cancer Treatment</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/pdq/treatment/endometrial/Patient</t>
+  </si>
+  <si>
+    <t>Clinical Trials to Treat Endometrial Cancer</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/clinicaltrials/search/results?protocolsearchid=6102305&amp;vers=1</t>
+  </si>
+  <si>
+    <t>Clinical Trials to Treat Uterine Sarcoma</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/clinicaltrials/search/results?protocolsearchid=13853828</t>
+  </si>
+  <si>
+    <t>Drugs Approved for Endometrial Cancer</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/druginfo/endometrialcancer</t>
+  </si>
+  <si>
+    <t>Endometrial Cancer Prevention</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/pdq/prevention/endometrial/Patient</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/pdq/prevention/endometrial/HealthProfessional</t>
+  </si>
+  <si>
+    <t>DOESN'T EXIST YET [cancer.gov/cancertopics/causes-prevention/risk-factors/hormones]</t>
+  </si>
+  <si>
+    <t>Endometrial Cancer Screening</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/pdq/screening/endometrial/Patient</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/pdq/screening/endometrial/HealthProfessional</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PDQ Screening Information </t>
+  </si>
+  <si>
+    <t>http://seer.cancer.gov/statfacts/html/corp.html</t>
+  </si>
+  <si>
+    <t>Vaginal Cancer Treatment</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/pdq/treatment/vaginal/Patient</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/pdq/treatment/vaginal/HealthProfessional</t>
+  </si>
+  <si>
+    <t>Drugs Approved for Vaginal Cancer</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/druginfo/vaginalcancer</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/causes-prevention/risk-factors/hormones/des-fact-sheet</t>
+  </si>
+  <si>
+    <t>Diethylstilbestrol (DES) and Cancer</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/pdq/treatment/vulvar/Patient</t>
+  </si>
+  <si>
+    <t>Vulvar Cancer Treatment</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/pdq/treatment/vulvar/HealthProfessional</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/druginfo/vulvarcancer</t>
+  </si>
+  <si>
+    <t>Drugs Approved for Vulvar Cancer</t>
+  </si>
+  <si>
+    <t>http://seer.cancer.gov/statfacts/html/vulva.html</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/pdq/treatment/lchistio/Patient</t>
+  </si>
+  <si>
+    <t>Langerhans Cell Histiocytosis Treatment</t>
+  </si>
+  <si>
+    <t>http://www.cancer.gov/cancertopics/pdq/treatment/lchistio/HealthProfessional</t>
   </si>
 </sst>
 </file>
@@ -2268,7 +2658,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="663">
+  <cellStyleXfs count="925">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2932,8 +3322,270 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3007,8 +3659,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="663">
+  <cellStyles count="925">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -3389,6 +4044,137 @@
     <cellStyle name="Followed Hyperlink" xfId="658" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="660" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="662" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="664" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="666" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="668" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="670" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="672" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="674" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="676" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="678" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="680" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="682" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="684" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="686" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="688" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="690" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="692" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="694" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="696" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="698" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="700" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="702" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="704" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="706" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="708" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="710" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="712" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="714" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="716" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="718" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="720" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="722" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="724" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="726" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="728" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="730" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="732" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="734" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="736" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="738" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="740" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="742" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="744" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="746" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="748" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="750" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="752" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="754" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="756" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="758" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="760" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="762" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="764" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="766" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="768" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="770" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="772" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="774" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="776" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="778" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="780" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="782" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="784" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="786" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="788" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="790" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="792" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="794" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="796" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="798" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="800" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="802" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="804" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="806" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="808" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="810" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="812" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="814" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="816" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="818" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="820" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="822" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="824" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="826" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="828" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="830" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="832" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="834" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="836" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="838" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="840" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="842" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="844" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="846" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="848" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="850" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="852" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="854" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="856" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="858" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="860" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="862" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="864" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="866" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="868" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="870" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="872" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="874" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="876" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="878" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="880" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="882" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="884" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="886" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="888" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="890" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="892" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="894" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="896" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="898" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="900" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="902" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="904" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="906" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="908" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="910" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="912" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="914" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="916" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="918" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="920" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="922" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="924" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -3671,6 +4457,137 @@
     <cellStyle name="Hyperlink" xfId="657" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="659" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="661" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="663" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="665" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="667" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="669" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="671" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="673" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="675" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="677" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="679" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="681" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="683" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="685" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="687" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="689" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="691" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="693" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="695" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="697" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="699" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="701" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="703" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="705" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="707" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="709" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="711" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="713" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="715" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="717" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="719" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="721" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="723" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="725" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="727" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="729" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="731" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="733" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="735" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="737" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="739" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="741" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="743" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="745" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="747" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="749" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="751" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="753" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="755" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="757" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="759" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="761" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="763" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="765" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="767" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="769" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="771" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="773" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="775" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="777" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="779" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="781" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="783" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="785" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="787" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="789" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="791" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="793" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="795" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="797" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="799" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="801" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="803" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="805" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="807" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="809" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="811" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="813" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="815" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="817" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="819" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="821" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="823" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="825" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="827" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="829" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="831" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="833" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="835" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="837" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="839" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="841" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="843" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="845" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="847" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="849" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="851" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="853" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="855" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="857" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="859" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="861" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="863" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="865" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="867" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="869" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="871" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="873" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="875" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="877" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="879" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="881" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="883" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="885" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="887" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="889" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="891" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="893" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="895" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="897" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="899" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="901" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="903" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="905" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="907" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="909" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="911" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="913" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="915" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="917" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="919" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="921" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="923" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -10858,7 +11775,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5:F5"/>
+      <selection pane="bottomLeft" activeCell="C9" activeCellId="2" sqref="C2 C4 C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -10897,7 +11814,7 @@
       <c r="B2" s="15" t="s">
         <v>560</v>
       </c>
-      <c r="C2" s="15"/>
+      <c r="C2" s="28"/>
       <c r="D2" s="15" t="s">
         <v>33</v>
       </c>
@@ -10933,7 +11850,7 @@
       <c r="B4" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="C4" s="15"/>
+      <c r="C4" s="28"/>
       <c r="D4" s="15" t="s">
         <v>29</v>
       </c>
@@ -11029,7 +11946,7 @@
       <c r="B9" s="15" t="s">
         <v>561</v>
       </c>
-      <c r="C9" s="15"/>
+      <c r="C9" s="28"/>
       <c r="D9" s="15" t="s">
         <v>33</v>
       </c>
@@ -13400,7 +14317,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="A4" sqref="A4:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -13679,9 +14596,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomLeft" activeCell="C10" activeCellId="3" sqref="C2 C5 C9 C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -13720,7 +14637,7 @@
       <c r="B2" s="15" t="s">
         <v>663</v>
       </c>
-      <c r="C2" s="15"/>
+      <c r="C2" s="28"/>
       <c r="D2" s="15" t="s">
         <v>33</v>
       </c>
@@ -13750,7 +14667,7 @@
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="43" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="42" t="s">
@@ -13766,6 +14683,540 @@
         <v>37</v>
       </c>
       <c r="F4" s="42" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="44" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>566</v>
+      </c>
+      <c r="C5" s="28"/>
+      <c r="D5" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" s="15">
+        <v>6158</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>519</v>
+      </c>
+      <c r="C7" s="15">
+        <v>899999</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" s="36" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" s="15">
+        <v>6145</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="15" t="s">
+        <v>664</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>665</v>
+      </c>
+      <c r="C9" s="28"/>
+      <c r="D9" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="15" t="s">
+        <v>669</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>668</v>
+      </c>
+      <c r="C10" s="28"/>
+      <c r="D10" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" s="15">
+        <v>1654</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="C12" s="15">
+        <v>1541</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="54.33203125" customWidth="1"/>
+    <col min="2" max="2" width="79.6640625" customWidth="1"/>
+    <col min="4" max="4" width="25.33203125" customWidth="1"/>
+    <col min="5" max="5" width="20.83203125" customWidth="1"/>
+    <col min="6" max="6" width="17" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="16">
+      <c r="A1" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="15" t="s">
+        <v>670</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>671</v>
+      </c>
+      <c r="C2" s="28"/>
+      <c r="D2" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="15" t="s">
+        <v>673</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>674</v>
+      </c>
+      <c r="C3" s="11"/>
+      <c r="D3" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="15" t="s">
+        <v>676</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>675</v>
+      </c>
+      <c r="C4" s="28"/>
+      <c r="D4" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>608</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="43" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="22">
+        <v>6835</v>
+      </c>
+      <c r="D5" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="22" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>566</v>
+      </c>
+      <c r="C6" s="28"/>
+      <c r="D6" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" s="15">
+        <v>6158</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>519</v>
+      </c>
+      <c r="C8" s="15">
+        <v>899999</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" s="36" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9" s="15">
+        <v>6145</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="15" t="s">
+        <v>670</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>672</v>
+      </c>
+      <c r="C10" s="28"/>
+      <c r="D10" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="15" t="s">
+        <v>678</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>677</v>
+      </c>
+      <c r="C11" s="28"/>
+      <c r="D11" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="C12" s="15">
+        <v>1654</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="C13" s="15">
+        <v>1541</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="43.33203125" customWidth="1"/>
+    <col min="2" max="2" width="74.83203125" customWidth="1"/>
+    <col min="4" max="4" width="30.83203125" customWidth="1"/>
+    <col min="5" max="5" width="25.6640625" customWidth="1"/>
+    <col min="6" max="6" width="17" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="16">
+      <c r="A1" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="15" t="s">
+        <v>680</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>679</v>
+      </c>
+      <c r="C2" s="28"/>
+      <c r="D2" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="15" t="s">
+        <v>683</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>682</v>
+      </c>
+      <c r="C3" s="11"/>
+      <c r="D3" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="43" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="22">
+        <v>6835</v>
+      </c>
+      <c r="D4" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="22" t="s">
         <v>39</v>
       </c>
     </row>
@@ -13776,7 +15227,7 @@
       <c r="B5" s="15" t="s">
         <v>566</v>
       </c>
-      <c r="C5" s="15"/>
+      <c r="C5" s="28"/>
       <c r="D5" s="15" t="s">
         <v>29</v>
       </c>
@@ -13849,12 +15300,12 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="15" t="s">
-        <v>664</v>
+        <v>680</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>665</v>
-      </c>
-      <c r="C9" s="15"/>
+        <v>681</v>
+      </c>
+      <c r="C9" s="28"/>
       <c r="D9" s="15" t="s">
         <v>33</v>
       </c>
@@ -13867,14 +15318,712 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="15" t="s">
-        <v>669</v>
+        <v>63</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" s="15">
+        <v>1654</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" s="15">
+        <v>1541</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="51.1640625" customWidth="1"/>
+    <col min="2" max="2" width="82.1640625" customWidth="1"/>
+    <col min="4" max="4" width="29.83203125" customWidth="1"/>
+    <col min="5" max="5" width="25.6640625" customWidth="1"/>
+    <col min="6" max="6" width="17.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="16">
+      <c r="A1" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="15" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>685</v>
+      </c>
+      <c r="C2" s="28"/>
+      <c r="D2" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="15" t="s">
+        <v>687</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>688</v>
+      </c>
+      <c r="C3" s="11"/>
+      <c r="D3" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="15" t="s">
+        <v>690</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>689</v>
+      </c>
+      <c r="C4" s="28"/>
+      <c r="D4" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="15" t="s">
+        <v>692</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>691</v>
+      </c>
+      <c r="C5" s="28"/>
+      <c r="D5" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="15" t="s">
+        <v>694</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>693</v>
+      </c>
+      <c r="C6" s="28"/>
+      <c r="D6" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="15" t="s">
+        <v>695</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>696</v>
+      </c>
+      <c r="C7" s="28"/>
+      <c r="D7" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="22">
+        <v>6835</v>
+      </c>
+      <c r="D8" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" s="22" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="15" t="s">
+        <v>444</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>697</v>
+      </c>
+      <c r="C9" s="28"/>
+      <c r="D9" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="15" t="s">
+        <v>6</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>668</v>
-      </c>
-      <c r="C10" s="15"/>
+        <v>566</v>
+      </c>
+      <c r="C10" s="28"/>
       <c r="D10" s="15" t="s">
         <v>29</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="14" t="s">
+        <v>698</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>699</v>
+      </c>
+      <c r="C11" s="28"/>
+      <c r="D11" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="14" t="s">
+        <v>702</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>701</v>
+      </c>
+      <c r="C12" s="28"/>
+      <c r="D12" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="14" t="s">
+        <v>705</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>704</v>
+      </c>
+      <c r="C13" s="11"/>
+      <c r="D13" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>519</v>
+      </c>
+      <c r="C14" s="15">
+        <v>899999</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F14" s="36" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="14" t="s">
+        <v>709</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>708</v>
+      </c>
+      <c r="C15" s="28"/>
+      <c r="D15" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="14" t="s">
+        <v>712</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>711</v>
+      </c>
+      <c r="C16" s="28"/>
+      <c r="D16" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="14" t="s">
+        <v>713</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>714</v>
+      </c>
+      <c r="C17" s="11"/>
+      <c r="D17" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="14" t="s">
+        <v>715</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>716</v>
+      </c>
+      <c r="C18" s="28"/>
+      <c r="D18" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="F18" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="15"/>
+      <c r="B19" s="15" t="s">
+        <v>717</v>
+      </c>
+      <c r="C19" s="11"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="F19" s="14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="15" t="s">
+        <v>684</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>686</v>
+      </c>
+      <c r="C20" s="28"/>
+      <c r="D20" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F20" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="15" t="s">
+        <v>698</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>700</v>
+      </c>
+      <c r="C21" s="28"/>
+      <c r="D21" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F21" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="14" t="s">
+        <v>702</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>703</v>
+      </c>
+      <c r="C22" s="28"/>
+      <c r="D22" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E22" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="F22" s="14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="14" t="s">
+        <v>707</v>
+      </c>
+      <c r="B23" s="15" t="s">
+        <v>706</v>
+      </c>
+      <c r="C23" s="28"/>
+      <c r="D23" s="14" t="s">
+        <v>391</v>
+      </c>
+      <c r="E23" s="14" t="s">
+        <v>288</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="14" t="s">
+        <v>709</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>710</v>
+      </c>
+      <c r="C24" s="28"/>
+      <c r="D24" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="E24" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="F24" s="14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" activeCellId="2" sqref="C2 C9 C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="52.5" customWidth="1"/>
+    <col min="2" max="2" width="76" customWidth="1"/>
+    <col min="4" max="4" width="28.83203125" customWidth="1"/>
+    <col min="5" max="5" width="24.83203125" customWidth="1"/>
+    <col min="6" max="6" width="14.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="16">
+      <c r="A1" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="15" t="s">
+        <v>718</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>719</v>
+      </c>
+      <c r="C2" s="28"/>
+      <c r="D2" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="15" t="s">
+        <v>657</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>658</v>
+      </c>
+      <c r="C3" s="28"/>
+      <c r="D3" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="22">
+        <v>6835</v>
+      </c>
+      <c r="D4" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="22" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>566</v>
+      </c>
+      <c r="C5" s="28"/>
+      <c r="D5" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" s="15">
+        <v>6158</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>519</v>
+      </c>
+      <c r="C7" s="15">
+        <v>899999</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" s="36" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" s="15">
+        <v>6145</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="15"/>
+      <c r="B9" s="15" t="s">
+        <v>721</v>
+      </c>
+      <c r="C9" s="28"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="15" t="s">
+        <v>718</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>720</v>
+      </c>
+      <c r="C10" s="28"/>
+      <c r="D10" s="15" t="s">
+        <v>33</v>
       </c>
       <c r="E10" s="15" t="s">
         <v>37</v>
@@ -13920,6 +16069,974 @@
         <v>44</v>
       </c>
       <c r="F12" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:F15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="39.1640625" customWidth="1"/>
+    <col min="2" max="2" width="86.33203125" customWidth="1"/>
+    <col min="4" max="4" width="25.1640625" customWidth="1"/>
+    <col min="5" max="5" width="25.83203125" customWidth="1"/>
+    <col min="6" max="6" width="18.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="16">
+      <c r="A1" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="15" t="s">
+        <v>722</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>723</v>
+      </c>
+      <c r="C2" s="28"/>
+      <c r="D2" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" s="14">
+        <v>2898</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="15" t="s">
+        <v>725</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>726</v>
+      </c>
+      <c r="C4" s="11"/>
+      <c r="D4" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="15" t="s">
+        <v>727</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>728</v>
+      </c>
+      <c r="C5" s="28"/>
+      <c r="D5" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="22">
+        <v>6835</v>
+      </c>
+      <c r="D6" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="22" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>566</v>
+      </c>
+      <c r="C7" s="28"/>
+      <c r="D7" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" s="15">
+        <v>6158</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="15" t="s">
+        <v>730</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>729</v>
+      </c>
+      <c r="C9" s="11"/>
+      <c r="D9" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>519</v>
+      </c>
+      <c r="C10" s="15">
+        <v>899999</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" s="36" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="14" t="s">
+        <v>731</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>732</v>
+      </c>
+      <c r="C11" s="28"/>
+      <c r="D11" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="14" t="s">
+        <v>734</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>528</v>
+      </c>
+      <c r="C12" s="28"/>
+      <c r="D12" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="15"/>
+      <c r="B13" s="15" t="s">
+        <v>735</v>
+      </c>
+      <c r="C13" s="11"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="15" t="s">
+        <v>722</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>724</v>
+      </c>
+      <c r="C14" s="28"/>
+      <c r="D14" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="C15" s="14">
+        <v>2840</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="C16" s="15">
+        <v>1654</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F16" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="15" t="s">
+        <v>731</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>733</v>
+      </c>
+      <c r="C17" s="28"/>
+      <c r="D17" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="F17" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="47" customWidth="1"/>
+    <col min="2" max="2" width="84.5" customWidth="1"/>
+    <col min="4" max="4" width="27.6640625" customWidth="1"/>
+    <col min="5" max="5" width="23.5" customWidth="1"/>
+    <col min="6" max="6" width="17.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="16">
+      <c r="A1" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="15" t="s">
+        <v>737</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>736</v>
+      </c>
+      <c r="C2" s="28"/>
+      <c r="D2" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" s="14">
+        <v>2898</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="15" t="s">
+        <v>740</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>739</v>
+      </c>
+      <c r="C4" s="11"/>
+      <c r="D4" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="22">
+        <v>6835</v>
+      </c>
+      <c r="D5" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="22" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>566</v>
+      </c>
+      <c r="C6" s="28"/>
+      <c r="D6" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" s="15">
+        <v>6158</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>519</v>
+      </c>
+      <c r="C8" s="15">
+        <v>899999</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" s="36" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9" s="15">
+        <v>6145</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="15" t="s">
+        <v>737</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>738</v>
+      </c>
+      <c r="C10" s="28"/>
+      <c r="D10" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="C11" s="14">
+        <v>2840</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="C12" s="15">
+        <v>1654</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="C13" s="15">
+        <v>1541</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="41.33203125" customWidth="1"/>
+    <col min="2" max="2" width="84.6640625" customWidth="1"/>
+    <col min="4" max="4" width="33.33203125" customWidth="1"/>
+    <col min="5" max="5" width="23.33203125" customWidth="1"/>
+    <col min="6" max="6" width="19.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="16">
+      <c r="A1" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="15" t="s">
+        <v>742</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>741</v>
+      </c>
+      <c r="C2" s="28"/>
+      <c r="D2" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" s="14">
+        <v>2898</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="15" t="s">
+        <v>745</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>744</v>
+      </c>
+      <c r="C4" s="45"/>
+      <c r="D4" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="15" t="s">
+        <v>746</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>747</v>
+      </c>
+      <c r="C5" s="28"/>
+      <c r="D5" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="15" t="s">
+        <v>748</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>749</v>
+      </c>
+      <c r="C6" s="28"/>
+      <c r="D6" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>566</v>
+      </c>
+      <c r="C7" s="28"/>
+      <c r="D7" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" s="15">
+        <v>6158</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="14" t="s">
+        <v>753</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>752</v>
+      </c>
+      <c r="C9" s="28"/>
+      <c r="D9" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" s="15">
+        <v>6145</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="15"/>
+      <c r="B11" s="15" t="s">
+        <v>754</v>
+      </c>
+      <c r="C11" s="11"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="15" t="s">
+        <v>742</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>743</v>
+      </c>
+      <c r="C12" s="28"/>
+      <c r="D12" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="C13" s="14">
+        <v>2840</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="15" t="s">
+        <v>669</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>668</v>
+      </c>
+      <c r="C14" s="28"/>
+      <c r="D14" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>608</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="C15" s="15">
+        <v>1654</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F15" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="15" t="s">
+        <v>751</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>750</v>
+      </c>
+      <c r="C16" s="28"/>
+      <c r="D16" s="15" t="s">
+        <v>391</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>288</v>
+      </c>
+      <c r="F16" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="C17" s="15">
+        <v>1541</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="F17" s="15" t="s">
         <v>40</v>
       </c>
     </row>
@@ -14279,6 +17396,1498 @@
         <v>40</v>
       </c>
       <c r="G16" s="15"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="34.1640625" customWidth="1"/>
+    <col min="2" max="2" width="70" customWidth="1"/>
+    <col min="4" max="4" width="26.6640625" customWidth="1"/>
+    <col min="5" max="5" width="28.6640625" customWidth="1"/>
+    <col min="6" max="6" width="16.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="16">
+      <c r="A1" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="15" t="s">
+        <v>757</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>755</v>
+      </c>
+      <c r="C2" s="28"/>
+      <c r="D2" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="15" t="s">
+        <v>657</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>658</v>
+      </c>
+      <c r="C3" s="28"/>
+      <c r="D3" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="22">
+        <v>6835</v>
+      </c>
+      <c r="D4" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="22" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>566</v>
+      </c>
+      <c r="C5" s="28"/>
+      <c r="D5" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" s="15">
+        <v>6158</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>519</v>
+      </c>
+      <c r="C7" s="15">
+        <v>899999</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" s="36" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" s="15">
+        <v>6145</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="15" t="s">
+        <v>757</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>756</v>
+      </c>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" s="15">
+        <v>1654</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" s="15">
+        <v>1541</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="47.33203125" customWidth="1"/>
+    <col min="2" max="2" width="79.83203125" customWidth="1"/>
+    <col min="4" max="4" width="30.83203125" customWidth="1"/>
+    <col min="5" max="5" width="24" customWidth="1"/>
+    <col min="6" max="6" width="21.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="16">
+      <c r="A1" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="15" t="s">
+        <v>758</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>759</v>
+      </c>
+      <c r="C2" s="28"/>
+      <c r="D2" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="15" t="s">
+        <v>763</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>764</v>
+      </c>
+      <c r="C3" s="28"/>
+      <c r="D3" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="15" t="s">
+        <v>767</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>768</v>
+      </c>
+      <c r="C4" s="11"/>
+      <c r="D4" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="15" t="s">
+        <v>765</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>766</v>
+      </c>
+      <c r="C5" s="11"/>
+      <c r="D5" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="15" t="s">
+        <v>769</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>770</v>
+      </c>
+      <c r="C6" s="28"/>
+      <c r="D6" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="22">
+        <v>6835</v>
+      </c>
+      <c r="D7" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" s="22" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>566</v>
+      </c>
+      <c r="C8" s="28"/>
+      <c r="D8" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="14" t="s">
+        <v>771</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>772</v>
+      </c>
+      <c r="C9" s="28"/>
+      <c r="D9" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="14" t="s">
+        <v>643</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>774</v>
+      </c>
+      <c r="C10" s="28"/>
+      <c r="D10" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="15" t="s">
+        <v>646</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>645</v>
+      </c>
+      <c r="C11" s="28"/>
+      <c r="D11" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="15" t="s">
+        <v>648</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>647</v>
+      </c>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="15" t="s">
+        <v>775</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>776</v>
+      </c>
+      <c r="C13" s="28"/>
+      <c r="D13" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="15" t="s">
+        <v>213</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>528</v>
+      </c>
+      <c r="C14" s="28"/>
+      <c r="D14" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="15"/>
+      <c r="B15" s="15" t="s">
+        <v>779</v>
+      </c>
+      <c r="C15" s="11"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="F15" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="15" t="s">
+        <v>758</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>760</v>
+      </c>
+      <c r="C16" s="28"/>
+      <c r="D16" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F16" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="15" t="s">
+        <v>762</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>761</v>
+      </c>
+      <c r="C17" s="28"/>
+      <c r="D17" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F17" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="15" t="s">
+        <v>771</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>773</v>
+      </c>
+      <c r="C18" s="28"/>
+      <c r="D18" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F18" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="15" t="s">
+        <v>775</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>777</v>
+      </c>
+      <c r="C19" s="28"/>
+      <c r="D19" s="15" t="s">
+        <v>778</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="F19" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:F17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="48.5" customWidth="1"/>
+    <col min="2" max="2" width="85.83203125" customWidth="1"/>
+    <col min="4" max="4" width="27.33203125" customWidth="1"/>
+    <col min="5" max="5" width="18.83203125" customWidth="1"/>
+    <col min="6" max="6" width="19.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="16">
+      <c r="A1" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="15" t="s">
+        <v>780</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>781</v>
+      </c>
+      <c r="C2" s="28"/>
+      <c r="D2" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" s="14">
+        <v>2898</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="15" t="s">
+        <v>657</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>658</v>
+      </c>
+      <c r="C4" s="28"/>
+      <c r="D4" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="15" t="s">
+        <v>783</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>784</v>
+      </c>
+      <c r="C5" s="28"/>
+      <c r="D5" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="22">
+        <v>6835</v>
+      </c>
+      <c r="D6" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="22" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="15" t="s">
+        <v>678</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>677</v>
+      </c>
+      <c r="C7" s="28"/>
+      <c r="D7" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>566</v>
+      </c>
+      <c r="C8" s="28"/>
+      <c r="D8" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" s="15">
+        <v>6158</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="14" t="s">
+        <v>643</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>774</v>
+      </c>
+      <c r="C10" s="28"/>
+      <c r="D10" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>519</v>
+      </c>
+      <c r="C11" s="15">
+        <v>899999</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" s="36" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12" s="15">
+        <v>6145</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="15" t="s">
+        <v>780</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>782</v>
+      </c>
+      <c r="C13" s="28"/>
+      <c r="D13" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="C14" s="14">
+        <v>2840</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="C15" s="15">
+        <v>1654</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F15" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="15" t="s">
+        <v>786</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>785</v>
+      </c>
+      <c r="C16" s="28"/>
+      <c r="D16" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="C17" s="15">
+        <v>1541</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="F17" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="38.5" customWidth="1"/>
+    <col min="2" max="2" width="70.1640625" customWidth="1"/>
+    <col min="4" max="4" width="31" customWidth="1"/>
+    <col min="5" max="5" width="26.6640625" customWidth="1"/>
+    <col min="6" max="6" width="17.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="16">
+      <c r="A1" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="15" t="s">
+        <v>788</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>787</v>
+      </c>
+      <c r="C2" s="28"/>
+      <c r="D2" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="15" t="s">
+        <v>657</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>658</v>
+      </c>
+      <c r="C3" s="28"/>
+      <c r="D3" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="15" t="s">
+        <v>791</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>790</v>
+      </c>
+      <c r="C4" s="28"/>
+      <c r="D4" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="22">
+        <v>6835</v>
+      </c>
+      <c r="D5" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="22" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="15" t="s">
+        <v>678</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>677</v>
+      </c>
+      <c r="C6" s="28"/>
+      <c r="D6" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>566</v>
+      </c>
+      <c r="C7" s="28"/>
+      <c r="D7" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" s="15">
+        <v>6158</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>519</v>
+      </c>
+      <c r="C9" s="15">
+        <v>899999</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" s="36" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" s="15">
+        <v>6145</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="15"/>
+      <c r="B11" s="15" t="s">
+        <v>792</v>
+      </c>
+      <c r="C11" s="28"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="15" t="s">
+        <v>788</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>789</v>
+      </c>
+      <c r="C12" s="28"/>
+      <c r="D12" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" s="15">
+        <v>1654</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="C14" s="15">
+        <v>1541</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="48.5" customWidth="1"/>
+    <col min="2" max="2" width="77.5" customWidth="1"/>
+    <col min="4" max="4" width="26" customWidth="1"/>
+    <col min="5" max="5" width="23.5" customWidth="1"/>
+    <col min="6" max="6" width="22.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="16">
+      <c r="A1" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="15" t="s">
+        <v>794</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>793</v>
+      </c>
+      <c r="C2" s="28"/>
+      <c r="D2" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="15" t="s">
+        <v>657</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>658</v>
+      </c>
+      <c r="C3" s="28"/>
+      <c r="D3" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="22">
+        <v>6835</v>
+      </c>
+      <c r="D4" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="22" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>566</v>
+      </c>
+      <c r="C5" s="28"/>
+      <c r="D5" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" s="15">
+        <v>6158</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>519</v>
+      </c>
+      <c r="C7" s="15">
+        <v>899999</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" s="36" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" s="15">
+        <v>6145</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="15" t="s">
+        <v>794</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>795</v>
+      </c>
+      <c r="C9" s="28"/>
+      <c r="D9" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" s="15">
+        <v>1654</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" s="15">
+        <v>1541</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>40</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
updating based on Min's db check: And below dependentID does not exist in QA.
4924
8036
8726
9507
915366
</commit_message>
<xml_diff>
--- a/Daisy-xls/IA/CTHP-Cards.xlsx
+++ b/Daisy-xls/IA/CTHP-Cards.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="2430" windowWidth="24120" windowHeight="13440" tabRatio="863" firstSheet="24" activeTab="34"/>
+    <workbookView xWindow="735" yWindow="2430" windowWidth="24120" windowHeight="13440" tabRatio="863" firstSheet="9" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="ADRENOCORTICAL CARCINOMA" sheetId="2" r:id="rId1"/>
@@ -54,7 +54,7 @@
     <sheet name="VAGINAL" sheetId="43" r:id="rId45"/>
     <sheet name="VULVAR" sheetId="44" r:id="rId46"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -7768,16 +7768,17 @@
   </sheetPr>
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A33" sqref="A33"/>
-      <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
+      <selection pane="bottomLeft" activeCell="D7" sqref="C7:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="26" customWidth="1"/>
-    <col min="3" max="3" width="83.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.875" customWidth="1"/>
+    <col min="2" max="2" width="7.5" customWidth="1"/>
+    <col min="3" max="3" width="65.25" customWidth="1"/>
     <col min="6" max="6" width="25" customWidth="1"/>
     <col min="7" max="7" width="20" customWidth="1"/>
     <col min="8" max="8" width="14.875" customWidth="1"/>
@@ -12555,15 +12556,15 @@
   <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A29" sqref="A29"/>
-      <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="18.875" style="4" customWidth="1"/>
-    <col min="3" max="3" width="62.625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="37.25" style="4" customWidth="1"/>
     <col min="4" max="4" width="22.625" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.625" style="4" customWidth="1"/>
     <col min="6" max="6" width="28" style="4" customWidth="1"/>
@@ -12611,7 +12612,7 @@
       <c r="D2" s="28">
         <v>883453</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="4">
         <v>915564</v>
       </c>
       <c r="F2" s="28" t="s">
@@ -12658,10 +12659,10 @@
       <c r="C4" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="49">
+      <c r="D4" s="52">
         <v>915365</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="4">
         <v>917550</v>
       </c>
       <c r="F4" s="28" t="s">
@@ -12842,7 +12843,7 @@
         <v>27</v>
       </c>
       <c r="D11" s="28">
-        <v>8036</v>
+        <v>312373</v>
       </c>
       <c r="E11" s="71" t="s">
         <v>848</v>
@@ -12933,9 +12934,9 @@
       </c>
       <c r="I14" s="28"/>
     </row>
-    <row r="15" spans="1:9" s="7" customFormat="1" ht="141.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="28"/>
-      <c r="B15" s="76" t="s">
+      <c r="B15" s="73" t="s">
         <v>932</v>
       </c>
       <c r="C15" s="28" t="s">
@@ -12989,7 +12990,7 @@
       <c r="C17" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="49">
+      <c r="D17" s="52">
         <v>14152</v>
       </c>
       <c r="E17" s="73">
@@ -13096,7 +13097,7 @@
         <v>15</v>
       </c>
       <c r="D21" s="24">
-        <v>9507</v>
+        <v>65193</v>
       </c>
       <c r="E21" s="71" t="s">
         <v>848</v>
@@ -13146,7 +13147,7 @@
         <v>19</v>
       </c>
       <c r="D23" s="24">
-        <v>4924</v>
+        <v>15732</v>
       </c>
       <c r="E23" s="73">
         <v>15505</v>
@@ -19263,7 +19264,7 @@
   </sheetPr>
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E8" sqref="E8"/>
       <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>

</xml_diff>